<commit_message>
Se avanza con el modelo relacional y las consultas de hasura, se avanza hasta compras
</commit_message>
<xml_diff>
--- a/ListadoQuerys.xlsx
+++ b/ListadoQuerys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectoPesLac\peslac-back\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47F1D80-81A5-49D7-AB1E-61E77E85B17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F16AB-AEDA-4F71-8A80-6D702A5A20A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AE78F90-65AD-4FFA-A2BC-D2300784A877}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="177">
   <si>
     <t>query ConsultaProductos {</t>
   </si>
@@ -106,9 +106,6 @@
     <t xml:space="preserve">    fecha_registro</t>
   </si>
   <si>
-    <t>Insert y Update Líneas producto</t>
-  </si>
-  <si>
     <t xml:space="preserve">  paquetes(where: {id: {_eq: 2}}) {</t>
   </si>
   <si>
@@ -172,15 +169,6 @@
     <t>query ConsultarPaquete {</t>
   </si>
   <si>
-    <t>Insert y Update Paquetes</t>
-  </si>
-  <si>
-    <t>Insert y Update Productos</t>
-  </si>
-  <si>
-    <t>Insert y Update proveedores</t>
-  </si>
-  <si>
     <t>query ConsultarProveedores {</t>
   </si>
   <si>
@@ -259,9 +247,6 @@
     <t xml:space="preserve">  update_clientes(where: {id: {_eq: $id}}, _set: $object) {</t>
   </si>
   <si>
-    <t>GET, Insert y Update clientes</t>
-  </si>
-  <si>
     <t>query ConsultarInventario {</t>
   </si>
   <si>
@@ -326,6 +311,261 @@
   </si>
   <si>
     <t xml:space="preserve">  insert_configuracion_paquetes_one(object: $object) {</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    returning{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     id </t>
+  </si>
+  <si>
+    <t>Se inserta un array de objetos adicionando el id insertado previamente</t>
+  </si>
+  <si>
+    <t>Se actualiza el inventario del producto por cada producto agregado, se debe envíar la cantidad en negativo</t>
+  </si>
+  <si>
+    <t>mutation ActualizarProductoInsertaHistorial($id_producto: Int = 10, $cantidad: Int = 10) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_historial_devoluciones_salidas_productos_one(object: {id_producto: $id_producto, id_tipo_operacion: 1, comentario: "Salida de producto por venta", cantidad: $cantidad}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cliente {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      nombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      apellidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    usuario {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        precio_venta</t>
+  </si>
+  <si>
+    <t>Historial Ventas</t>
+  </si>
+  <si>
+    <t>Informe de ventas general</t>
+  </si>
+  <si>
+    <t>query InformeVentasGeneral($fechaInicio: date = "2022-07-02", $fechaFin: date = "2022-07-03") {</t>
+  </si>
+  <si>
+    <t>Informe de ventas detallado</t>
+  </si>
+  <si>
+    <t>query InformeVentasDetallado($fechaInicio: date = "2022-07-02", $fechaFin: date = "2022-07-03") {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    venta {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      cliente {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        nombres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        apellidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      lineas_producto {</t>
+  </si>
+  <si>
+    <t>Consulta detalle de venta</t>
+  </si>
+  <si>
+    <t>query ConsultarDetalleVenta($idVenta: Int = 4) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ventas(where: {id: {_eq: $idVenta}}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      estacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      nit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    metodos_pago {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    consecutivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        lineas_producto {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        valor_inpuesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      total</t>
+  </si>
+  <si>
+    <t>mutation InsertarDevolucion($cantidad: Int = 1, $id_producto: Int = 2, $id_tipo_operacion: Int = 2, $comentario: String = "") {</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>mutation AnularVenta($id_venta: Int = 10, $comentario: String = "") {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_ventas_anuladas_one(object: {id_venta: $id_venta, comentario: $comentario}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  update_ventas(where: {id: {_eq: $id_venta}}, _set: {anulado: true}) {</t>
+  </si>
+  <si>
+    <t>Anular Venta.. Despues de ejecutar, hay que actualziar la vista principal</t>
+  </si>
+  <si>
+    <t>query VentasAnuladas($fechaInicio: date = "2022-07-02", $fechaFin: date = "2022-07-03") {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ventas_anuladas(where: {fecha_registro: {_gte: $fechaInicio, _lte: $fechaFin}}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      fecha_registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      usuario {</t>
+  </si>
+  <si>
+    <t>Consulta de Ventas anuladas</t>
+  </si>
+  <si>
+    <t>Paquetes</t>
+  </si>
+  <si>
+    <t>Lineas Producto</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Se inserta la orden y se obtiene el ID</t>
+  </si>
+  <si>
+    <t>mutation InsertarOrden($object: ordenes_insert_input!) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_ordenes_one(object: $object) {</t>
+  </si>
+  <si>
+    <t>mutation InsertarVenta($id_orden: Int = 10) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_ventas_one(object: {id_orden: $id_orden}) {</t>
+  </si>
+  <si>
+    <t>Se inserta la venta</t>
+  </si>
+  <si>
+    <t>mutation InsertarDetalleOrden($object: [detalle_ordenes_insert_input!]!) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_detalle_ordenes(objects: $object) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    detalle_ordenes {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ordene {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      detalle_ordenes {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        cantidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        producto {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          precio_venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  detalle_ordenes(where: {ordene: {ventas: {fecha_registro: {_gte: $fechaInicio, _lte: $fechaFin}}}}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ordene{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ventas(order_by: {id: asc}, where: {ordene: {fecha_registro: {_gte: $fechaInicio, _lte: $fechaFin}}, anulado: {_eq: false}}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ordene{</t>
+  </si>
+  <si>
+    <t>Para devolución se usa la mutación de inventario</t>
+  </si>
+  <si>
+    <t>Compras</t>
+  </si>
+  <si>
+    <t>Se inserta la compra</t>
+  </si>
+  <si>
+    <t>mutation InsertarCompra($id_orden: Int = 10, $id_proveedor: Int = 10) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_compras_one(object: {id_orden: $id_orden, id_estado_compra: 1, id_proveedor: $id_proveedor}) {</t>
+  </si>
+  <si>
+    <t>query ConsultarCuentasPorPagar {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  compras {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    proveedore {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      detalle_ordenes_aggregate {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        aggregate {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          sum {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          }</t>
+  </si>
+  <si>
+    <t>Consulta Cuentas por pagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  insert_historial_devoluciones_salidas_productos_one(object: {id_producto: $id_producto, id_tipo_operacion: 1, comentario: "Salida de producto por compra", cantidad: $cantidad}) {</t>
   </si>
 </sst>
 </file>
@@ -349,7 +589,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +620,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -393,16 +639,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,24 +975,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E99040-D82E-45BB-95AB-EA9D37042862}">
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:P436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
+      <selection activeCell="A414" sqref="A414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="A1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -956,7 +1214,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -967,7 +1225,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1020,7 +1278,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1031,7 +1289,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1105,15 +1363,15 @@
       <c r="G35" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="A37" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -1126,7 +1384,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1137,7 +1395,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1199,7 +1457,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1210,7 +1468,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1284,15 +1542,15 @@
       <c r="G53" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
+      <c r="A58" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -1305,7 +1563,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1316,7 +1574,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1378,7 +1636,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1389,7 +1647,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1442,7 +1700,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1453,7 +1711,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1486,7 +1744,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1508,7 +1766,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -1519,7 +1777,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -1530,7 +1788,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -1541,7 +1799,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -1552,7 +1810,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -1563,7 +1821,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -1574,7 +1832,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -1585,7 +1843,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -1596,7 +1854,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -1607,7 +1865,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -1618,7 +1876,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -1629,7 +1887,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -1640,7 +1898,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -1662,7 +1920,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -1673,7 +1931,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -1684,7 +1942,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -1695,7 +1953,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -1706,7 +1964,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -1717,7 +1975,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -1769,19 +2027,19 @@
       <c r="G102" s="2"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
+      <c r="A105" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -1792,7 +2050,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -1814,7 +2072,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -1836,7 +2094,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -1847,7 +2105,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -1858,7 +2116,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -1869,7 +2127,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -1880,7 +2138,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -1891,7 +2149,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -1902,7 +2160,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -1913,7 +2171,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -1964,7 +2222,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -1975,7 +2233,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2028,7 +2286,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2039,7 +2297,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2104,321 +2362,321 @@
       <c r="G135" s="3"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
-      <c r="G140" s="4"/>
+      <c r="A140" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="6"/>
+      <c r="F140" s="6"/>
+      <c r="G140" s="6"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+      <c r="A141" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B141" s="4"/>
+      <c r="C141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B141" s="5"/>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5"/>
-      <c r="E141" s="5"/>
-      <c r="F141" s="5"/>
-      <c r="G141" s="5"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+      <c r="B146" s="4"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="4"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="4"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B142" s="5"/>
-      <c r="C142" s="5"/>
-      <c r="D142" s="5"/>
-      <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
-      <c r="G142" s="5"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
+      <c r="B148" s="4"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="4"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B155" s="4"/>
+      <c r="C155" s="4"/>
+      <c r="D155" s="4"/>
+      <c r="E155" s="4"/>
+      <c r="F155" s="4"/>
+      <c r="G155" s="4"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B143" s="5"/>
-      <c r="C143" s="5"/>
-      <c r="D143" s="5"/>
-      <c r="E143" s="5"/>
-      <c r="F143" s="5"/>
-      <c r="G143" s="5"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B144" s="5"/>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
-      <c r="G144" s="5"/>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B145" s="5"/>
-      <c r="C145" s="5"/>
-      <c r="D145" s="5"/>
-      <c r="E145" s="5"/>
-      <c r="F145" s="5"/>
-      <c r="G145" s="5"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B146" s="5"/>
-      <c r="C146" s="5"/>
-      <c r="D146" s="5"/>
-      <c r="E146" s="5"/>
-      <c r="F146" s="5"/>
-      <c r="G146" s="5"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B147" s="5"/>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="5"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
+      <c r="B157" s="4"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="4"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="4"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B158" s="4"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="4"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4"/>
+      <c r="G158" s="4"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="4"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4"/>
+      <c r="G159" s="4"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="4"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4"/>
+      <c r="G160" s="4"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B148" s="5"/>
-      <c r="C148" s="5"/>
-      <c r="D148" s="5"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="5"/>
-      <c r="G148" s="5"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B149" s="5"/>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="5"/>
-      <c r="G149" s="5"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="4"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B150" s="5"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
-      <c r="G150" s="5"/>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
+      <c r="B162" s="4"/>
+      <c r="C162" s="4"/>
+      <c r="D162" s="4"/>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="4"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B164" s="4"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="4"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B151" s="5"/>
-      <c r="C151" s="5"/>
-      <c r="D151" s="5"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="5"/>
-      <c r="G151" s="5"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B152" s="5"/>
-      <c r="C152" s="5"/>
-      <c r="D152" s="5"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="5"/>
-      <c r="G152" s="5"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="5"/>
-      <c r="B153" s="5"/>
-      <c r="C153" s="5"/>
-      <c r="D153" s="5"/>
-      <c r="E153" s="5"/>
-      <c r="F153" s="5"/>
-      <c r="G153" s="5"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="5"/>
-      <c r="B154" s="5"/>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="5"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B155" s="5"/>
-      <c r="C155" s="5"/>
-      <c r="D155" s="5"/>
-      <c r="E155" s="5"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="5"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B156" s="5"/>
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
-      <c r="F156" s="5"/>
-      <c r="G156" s="5"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B157" s="5"/>
-      <c r="C157" s="5"/>
-      <c r="D157" s="5"/>
-      <c r="E157" s="5"/>
-      <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B158" s="5"/>
-      <c r="C158" s="5"/>
-      <c r="D158" s="5"/>
-      <c r="E158" s="5"/>
-      <c r="F158" s="5"/>
-      <c r="G158" s="5"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B159" s="5"/>
-      <c r="C159" s="5"/>
-      <c r="D159" s="5"/>
-      <c r="E159" s="5"/>
-      <c r="F159" s="5"/>
-      <c r="G159" s="5"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="5"/>
-      <c r="B160" s="5"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B161" s="5"/>
-      <c r="C161" s="5"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="5"/>
-      <c r="F161" s="5"/>
-      <c r="G161" s="5"/>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B162" s="5"/>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B163" s="5"/>
-      <c r="C163" s="5"/>
-      <c r="D163" s="5"/>
-      <c r="E163" s="5"/>
-      <c r="F163" s="5"/>
-      <c r="G163" s="5"/>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B164" s="5"/>
-      <c r="C164" s="5"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
-      <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B165" s="5"/>
-      <c r="C165" s="5"/>
-      <c r="D165" s="5"/>
-      <c r="E165" s="5"/>
-      <c r="F165" s="5"/>
-      <c r="G165" s="5"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B166" s="5"/>
-      <c r="C166" s="5"/>
-      <c r="D166" s="5"/>
-      <c r="E166" s="5"/>
-      <c r="F166" s="5"/>
-      <c r="G166" s="5"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B167" s="5"/>
-      <c r="C167" s="5"/>
-      <c r="D167" s="5"/>
-      <c r="E167" s="5"/>
-      <c r="F167" s="5"/>
-      <c r="G167" s="5"/>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
-      <c r="D172" s="4"/>
-      <c r="E172" s="4"/>
-      <c r="F172" s="4"/>
-      <c r="G172" s="4"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2505,8 +2763,8 @@
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="6" t="s">
-        <v>78</v>
+      <c r="A181" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -2517,7 +2775,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -2528,7 +2786,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -2561,7 +2819,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -2635,8 +2893,8 @@
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A193" s="6" t="s">
-        <v>79</v>
+      <c r="A193" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -2647,7 +2905,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -2658,7 +2916,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -2691,7 +2949,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -2766,7 +3024,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -2777,7 +3035,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -2810,7 +3068,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -2821,7 +3079,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -2854,7 +3112,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -2885,9 +3143,2400 @@
       <c r="F215" s="1"/>
       <c r="G215" s="1"/>
     </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="6"/>
+      <c r="E218" s="6"/>
+      <c r="F218" s="6"/>
+      <c r="G218" s="6"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B219" s="3"/>
+      <c r="C219" s="3"/>
+      <c r="D219" s="3"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B220" s="3"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B221" s="3"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B222" s="3"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B224" s="3"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B225" s="3"/>
+      <c r="C225" s="3"/>
+      <c r="D225" s="3"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B226" s="3"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B227" s="3"/>
+      <c r="C227" s="3"/>
+      <c r="D227" s="3"/>
+      <c r="E227" s="3"/>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B228" s="3"/>
+      <c r="C228" s="3"/>
+      <c r="D228" s="3"/>
+      <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B229" s="3"/>
+      <c r="C229" s="3"/>
+      <c r="D229" s="3"/>
+      <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B230" s="3"/>
+      <c r="C230" s="3"/>
+      <c r="D230" s="3"/>
+      <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B231" s="3"/>
+      <c r="C231" s="3"/>
+      <c r="D231" s="3"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B232" s="3"/>
+      <c r="C232" s="3"/>
+      <c r="D232" s="3"/>
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="3"/>
+      <c r="B233" s="3"/>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B234" s="3"/>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B239" s="3"/>
+      <c r="C239" s="3"/>
+      <c r="D239" s="3"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="3"/>
+      <c r="B240" s="3"/>
+      <c r="C240" s="3"/>
+      <c r="D240" s="3"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="3"/>
+      <c r="B241" s="3"/>
+      <c r="C241" s="3"/>
+      <c r="D241" s="3"/>
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="3"/>
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B243" s="3"/>
+      <c r="C243" s="3"/>
+      <c r="D243" s="3"/>
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B244" s="3"/>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B245" s="3"/>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B246" s="3"/>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B247" s="3"/>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B248" s="3"/>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B249" s="3"/>
+      <c r="C249" s="3"/>
+      <c r="D249" s="3"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B250" s="3"/>
+      <c r="C250" s="3"/>
+      <c r="D250" s="3"/>
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3"/>
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B252" s="3"/>
+      <c r="C252" s="3"/>
+      <c r="D252" s="3"/>
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B253" s="3"/>
+      <c r="C253" s="3"/>
+      <c r="D253" s="3"/>
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="3"/>
+      <c r="B254" s="3"/>
+      <c r="C254" s="3"/>
+      <c r="D254" s="3"/>
+      <c r="E254" s="3"/>
+      <c r="F254" s="3"/>
+      <c r="G254" s="3"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B258" s="6"/>
+      <c r="C258" s="6"/>
+      <c r="D258" s="6"/>
+      <c r="E258" s="6"/>
+      <c r="F258" s="6"/>
+      <c r="G258" s="6"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B259" s="8"/>
+      <c r="C259" s="8"/>
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="9"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B260" s="10"/>
+      <c r="C260" s="10"/>
+      <c r="D260" s="10"/>
+      <c r="E260" s="10"/>
+      <c r="F260" s="10"/>
+      <c r="G260" s="10"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B261" s="10"/>
+      <c r="C261" s="10"/>
+      <c r="D261" s="10"/>
+      <c r="E261" s="10"/>
+      <c r="F261" s="10"/>
+      <c r="G261" s="10"/>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B262" s="10"/>
+      <c r="C262" s="10"/>
+      <c r="D262" s="10"/>
+      <c r="E262" s="10"/>
+      <c r="F262" s="10"/>
+      <c r="G262" s="10"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B263" s="10"/>
+      <c r="C263" s="10"/>
+      <c r="D263" s="10"/>
+      <c r="E263" s="10"/>
+      <c r="F263" s="10"/>
+      <c r="G263" s="10"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B264" s="10"/>
+      <c r="C264" s="10"/>
+      <c r="D264" s="10"/>
+      <c r="E264" s="10"/>
+      <c r="F264" s="10"/>
+      <c r="G264" s="10"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B265" s="10"/>
+      <c r="C265" s="10"/>
+      <c r="D265" s="10"/>
+      <c r="E265" s="10"/>
+      <c r="F265" s="10"/>
+      <c r="G265" s="10"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B266" s="10"/>
+      <c r="C266" s="10"/>
+      <c r="D266" s="10"/>
+      <c r="E266" s="10"/>
+      <c r="F266" s="10"/>
+      <c r="G266" s="10"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B267" s="10"/>
+      <c r="C267" s="10"/>
+      <c r="D267" s="10"/>
+      <c r="E267" s="10"/>
+      <c r="F267" s="10"/>
+      <c r="G267" s="10"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B268" s="10"/>
+      <c r="C268" s="10"/>
+      <c r="D268" s="10"/>
+      <c r="E268" s="10"/>
+      <c r="F268" s="10"/>
+      <c r="G268" s="10"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B269" s="10"/>
+      <c r="C269" s="10"/>
+      <c r="D269" s="10"/>
+      <c r="E269" s="10"/>
+      <c r="F269" s="10"/>
+      <c r="G269" s="10"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B270" s="10"/>
+      <c r="C270" s="10"/>
+      <c r="D270" s="10"/>
+      <c r="E270" s="10"/>
+      <c r="F270" s="10"/>
+      <c r="G270" s="10"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B271" s="10"/>
+      <c r="C271" s="10"/>
+      <c r="D271" s="10"/>
+      <c r="E271" s="10"/>
+      <c r="F271" s="10"/>
+      <c r="G271" s="10"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B272" s="10"/>
+      <c r="C272" s="10"/>
+      <c r="D272" s="10"/>
+      <c r="E272" s="10"/>
+      <c r="F272" s="10"/>
+      <c r="G272" s="10"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B273" s="10"/>
+      <c r="C273" s="10"/>
+      <c r="D273" s="10"/>
+      <c r="E273" s="10"/>
+      <c r="F273" s="10"/>
+      <c r="G273" s="10"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B274" s="10"/>
+      <c r="C274" s="10"/>
+      <c r="D274" s="10"/>
+      <c r="E274" s="10"/>
+      <c r="F274" s="10"/>
+      <c r="G274" s="10"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B275" s="10"/>
+      <c r="C275" s="10"/>
+      <c r="D275" s="10"/>
+      <c r="E275" s="10"/>
+      <c r="F275" s="10"/>
+      <c r="G275" s="10"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B276" s="10"/>
+      <c r="C276" s="10"/>
+      <c r="D276" s="10"/>
+      <c r="E276" s="10"/>
+      <c r="F276" s="10"/>
+      <c r="G276" s="10"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B277" s="10"/>
+      <c r="C277" s="10"/>
+      <c r="D277" s="10"/>
+      <c r="E277" s="10"/>
+      <c r="F277" s="10"/>
+      <c r="G277" s="10"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B278" s="10"/>
+      <c r="C278" s="10"/>
+      <c r="D278" s="10"/>
+      <c r="E278" s="10"/>
+      <c r="F278" s="10"/>
+      <c r="G278" s="10"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B279" s="10"/>
+      <c r="C279" s="10"/>
+      <c r="D279" s="10"/>
+      <c r="E279" s="10"/>
+      <c r="F279" s="10"/>
+      <c r="G279" s="10"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B280" s="10"/>
+      <c r="C280" s="10"/>
+      <c r="D280" s="10"/>
+      <c r="E280" s="10"/>
+      <c r="F280" s="10"/>
+      <c r="G280" s="10"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B281" s="10"/>
+      <c r="C281" s="10"/>
+      <c r="D281" s="10"/>
+      <c r="E281" s="10"/>
+      <c r="F281" s="10"/>
+      <c r="G281" s="10"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="10"/>
+      <c r="B282" s="10"/>
+      <c r="C282" s="10"/>
+      <c r="D282" s="10"/>
+      <c r="E282" s="10"/>
+      <c r="F282" s="10"/>
+      <c r="G282" s="10"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="10"/>
+      <c r="B283" s="10"/>
+      <c r="C283" s="10"/>
+      <c r="D283" s="10"/>
+      <c r="E283" s="10"/>
+      <c r="F283" s="10"/>
+      <c r="G283" s="10"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B284" s="8"/>
+      <c r="C284" s="8"/>
+      <c r="D284" s="10"/>
+      <c r="E284" s="10"/>
+      <c r="F284" s="10"/>
+      <c r="G284" s="10"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B285" s="10"/>
+      <c r="C285" s="10"/>
+      <c r="D285" s="10"/>
+      <c r="E285" s="10"/>
+      <c r="F285" s="10"/>
+      <c r="G285" s="10"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B286" s="10"/>
+      <c r="C286" s="10"/>
+      <c r="D286" s="10"/>
+      <c r="E286" s="10"/>
+      <c r="F286" s="10"/>
+      <c r="G286" s="10"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B287" s="10"/>
+      <c r="C287" s="10"/>
+      <c r="D287" s="10"/>
+      <c r="E287" s="10"/>
+      <c r="F287" s="10"/>
+      <c r="G287" s="10"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B288" s="10"/>
+      <c r="C288" s="10"/>
+      <c r="D288" s="10"/>
+      <c r="E288" s="10"/>
+      <c r="F288" s="10"/>
+      <c r="G288" s="10"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B289" s="10"/>
+      <c r="C289" s="10"/>
+      <c r="D289" s="10"/>
+      <c r="E289" s="10"/>
+      <c r="F289" s="10"/>
+      <c r="G289" s="10"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B290" s="10"/>
+      <c r="C290" s="10"/>
+      <c r="D290" s="10"/>
+      <c r="E290" s="10"/>
+      <c r="F290" s="10"/>
+      <c r="G290" s="10"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B291" s="10"/>
+      <c r="C291" s="10"/>
+      <c r="D291" s="10"/>
+      <c r="E291" s="10"/>
+      <c r="F291" s="10"/>
+      <c r="G291" s="10"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B292" s="10"/>
+      <c r="C292" s="10"/>
+      <c r="D292" s="10"/>
+      <c r="E292" s="10"/>
+      <c r="F292" s="10"/>
+      <c r="G292" s="10"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B293" s="10"/>
+      <c r="C293" s="10"/>
+      <c r="D293" s="10"/>
+      <c r="E293" s="10"/>
+      <c r="F293" s="10"/>
+      <c r="G293" s="10"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B294" s="10"/>
+      <c r="C294" s="10"/>
+      <c r="D294" s="10"/>
+      <c r="E294" s="10"/>
+      <c r="F294" s="10"/>
+      <c r="G294" s="10"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B295" s="10"/>
+      <c r="C295" s="10"/>
+      <c r="D295" s="10"/>
+      <c r="E295" s="10"/>
+      <c r="F295" s="10"/>
+      <c r="G295" s="10"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B296" s="10"/>
+      <c r="C296" s="10"/>
+      <c r="D296" s="10"/>
+      <c r="E296" s="10"/>
+      <c r="F296" s="10"/>
+      <c r="G296" s="10"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B297" s="10"/>
+      <c r="C297" s="10"/>
+      <c r="D297" s="10"/>
+      <c r="E297" s="10"/>
+      <c r="F297" s="10"/>
+      <c r="G297" s="10"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B298" s="10"/>
+      <c r="C298" s="10"/>
+      <c r="D298" s="10"/>
+      <c r="E298" s="10"/>
+      <c r="F298" s="10"/>
+      <c r="G298" s="10"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B299" s="10"/>
+      <c r="C299" s="10"/>
+      <c r="D299" s="10"/>
+      <c r="E299" s="10"/>
+      <c r="F299" s="10"/>
+      <c r="G299" s="10"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B300" s="10"/>
+      <c r="C300" s="10"/>
+      <c r="D300" s="10"/>
+      <c r="E300" s="10"/>
+      <c r="F300" s="10"/>
+      <c r="G300" s="10"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B301" s="10"/>
+      <c r="C301" s="10"/>
+      <c r="D301" s="10"/>
+      <c r="E301" s="10"/>
+      <c r="F301" s="10"/>
+      <c r="G301" s="10"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B302" s="10"/>
+      <c r="C302" s="10"/>
+      <c r="D302" s="10"/>
+      <c r="E302" s="10"/>
+      <c r="F302" s="10"/>
+      <c r="G302" s="10"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B303" s="10"/>
+      <c r="C303" s="10"/>
+      <c r="D303" s="10"/>
+      <c r="E303" s="10"/>
+      <c r="F303" s="10"/>
+      <c r="G303" s="10"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="10"/>
+      <c r="B304" s="10"/>
+      <c r="C304" s="10"/>
+      <c r="D304" s="10"/>
+      <c r="E304" s="10"/>
+      <c r="F304" s="10"/>
+      <c r="G304" s="10"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B305" s="11"/>
+      <c r="C305" s="11"/>
+      <c r="D305" s="10"/>
+      <c r="E305" s="10"/>
+      <c r="F305" s="10"/>
+      <c r="G305" s="10"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B306" s="10"/>
+      <c r="C306" s="10"/>
+      <c r="D306" s="10"/>
+      <c r="E306" s="10"/>
+      <c r="F306" s="10"/>
+      <c r="G306" s="10"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B307" s="10"/>
+      <c r="C307" s="10"/>
+      <c r="D307" s="10"/>
+      <c r="E307" s="10"/>
+      <c r="F307" s="10"/>
+      <c r="G307" s="10"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B308" s="10"/>
+      <c r="C308" s="10"/>
+      <c r="D308" s="10"/>
+      <c r="E308" s="10"/>
+      <c r="F308" s="10"/>
+      <c r="G308" s="10"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B309" s="10"/>
+      <c r="C309" s="10"/>
+      <c r="D309" s="10"/>
+      <c r="E309" s="10"/>
+      <c r="F309" s="10"/>
+      <c r="G309" s="10"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B310" s="10"/>
+      <c r="C310" s="10"/>
+      <c r="D310" s="10"/>
+      <c r="E310" s="10"/>
+      <c r="F310" s="10"/>
+      <c r="G310" s="10"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B311" s="10"/>
+      <c r="C311" s="10"/>
+      <c r="D311" s="10"/>
+      <c r="E311" s="10"/>
+      <c r="F311" s="10"/>
+      <c r="G311" s="10"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B312" s="10"/>
+      <c r="C312" s="10"/>
+      <c r="D312" s="10"/>
+      <c r="E312" s="10"/>
+      <c r="F312" s="10"/>
+      <c r="G312" s="10"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B313" s="10"/>
+      <c r="C313" s="10"/>
+      <c r="D313" s="10"/>
+      <c r="E313" s="10"/>
+      <c r="F313" s="10"/>
+      <c r="G313" s="10"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B314" s="10"/>
+      <c r="C314" s="10"/>
+      <c r="D314" s="10"/>
+      <c r="E314" s="10"/>
+      <c r="F314" s="10"/>
+      <c r="G314" s="10"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B315" s="10"/>
+      <c r="C315" s="10"/>
+      <c r="D315" s="10"/>
+      <c r="E315" s="10"/>
+      <c r="F315" s="10"/>
+      <c r="G315" s="10"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B316" s="10"/>
+      <c r="C316" s="10"/>
+      <c r="D316" s="10"/>
+      <c r="E316" s="10"/>
+      <c r="F316" s="10"/>
+      <c r="G316" s="10"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B317" s="10"/>
+      <c r="C317" s="10"/>
+      <c r="D317" s="10"/>
+      <c r="E317" s="10"/>
+      <c r="F317" s="10"/>
+      <c r="G317" s="10"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B318" s="10"/>
+      <c r="C318" s="10"/>
+      <c r="D318" s="10"/>
+      <c r="E318" s="10"/>
+      <c r="F318" s="10"/>
+      <c r="G318" s="10"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B319" s="10"/>
+      <c r="C319" s="10"/>
+      <c r="D319" s="10"/>
+      <c r="E319" s="10"/>
+      <c r="F319" s="10"/>
+      <c r="G319" s="10"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B320" s="10"/>
+      <c r="C320" s="10"/>
+      <c r="D320" s="10"/>
+      <c r="E320" s="10"/>
+      <c r="F320" s="10"/>
+      <c r="G320" s="10"/>
+    </row>
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A321" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B321" s="10"/>
+      <c r="C321" s="10"/>
+      <c r="D321" s="10"/>
+      <c r="E321" s="10"/>
+      <c r="F321" s="10"/>
+      <c r="G321" s="10"/>
+    </row>
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A322" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B322" s="10"/>
+      <c r="C322" s="10"/>
+      <c r="D322" s="10"/>
+      <c r="E322" s="10"/>
+      <c r="F322" s="10"/>
+      <c r="G322" s="10"/>
+    </row>
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A323" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B323" s="10"/>
+      <c r="C323" s="10"/>
+      <c r="D323" s="10"/>
+      <c r="E323" s="10"/>
+      <c r="F323" s="10"/>
+      <c r="G323" s="10"/>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A324" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B324" s="10"/>
+      <c r="C324" s="10"/>
+      <c r="D324" s="10"/>
+      <c r="E324" s="10"/>
+      <c r="F324" s="10"/>
+      <c r="G324" s="10"/>
+    </row>
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A325" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B325" s="10"/>
+      <c r="C325" s="10"/>
+      <c r="D325" s="10"/>
+      <c r="E325" s="10"/>
+      <c r="F325" s="10"/>
+      <c r="G325" s="10"/>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A326" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B326" s="10"/>
+      <c r="C326" s="10"/>
+      <c r="D326" s="10"/>
+      <c r="E326" s="10"/>
+      <c r="F326" s="10"/>
+      <c r="G326" s="10"/>
+    </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A327" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B327" s="10"/>
+      <c r="C327" s="10"/>
+      <c r="D327" s="10"/>
+      <c r="E327" s="10"/>
+      <c r="F327" s="10"/>
+      <c r="G327" s="10"/>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A328" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B328" s="10"/>
+      <c r="C328" s="10"/>
+      <c r="D328" s="10"/>
+      <c r="E328" s="10"/>
+      <c r="F328" s="10"/>
+      <c r="G328" s="10"/>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A329" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B329" s="10"/>
+      <c r="C329" s="10"/>
+      <c r="D329" s="10"/>
+      <c r="E329" s="10"/>
+      <c r="F329" s="10"/>
+      <c r="G329" s="10"/>
+    </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A330" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B330" s="10"/>
+      <c r="C330" s="10"/>
+      <c r="D330" s="10"/>
+      <c r="E330" s="10"/>
+      <c r="F330" s="10"/>
+      <c r="G330" s="10"/>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A331" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B331" s="10"/>
+      <c r="C331" s="10"/>
+      <c r="D331" s="10"/>
+      <c r="E331" s="10"/>
+      <c r="F331" s="10"/>
+      <c r="G331" s="10"/>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A332" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B332" s="10"/>
+      <c r="C332" s="10"/>
+      <c r="D332" s="10"/>
+      <c r="E332" s="10"/>
+      <c r="F332" s="10"/>
+      <c r="G332" s="10"/>
+    </row>
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A333" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B333" s="10"/>
+      <c r="C333" s="10"/>
+      <c r="D333" s="10"/>
+      <c r="E333" s="10"/>
+      <c r="F333" s="10"/>
+      <c r="G333" s="10"/>
+      <c r="L333" s="13"/>
+      <c r="M333" s="13"/>
+      <c r="N333" s="13"/>
+      <c r="O333" s="13"/>
+      <c r="P333" s="13"/>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A334" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B334" s="10"/>
+      <c r="C334" s="10"/>
+      <c r="D334" s="10"/>
+      <c r="E334" s="10"/>
+      <c r="F334" s="10"/>
+      <c r="G334" s="10"/>
+      <c r="L334" s="13"/>
+      <c r="M334" s="13"/>
+      <c r="N334" s="13"/>
+      <c r="O334" s="13"/>
+      <c r="P334" s="13"/>
+    </row>
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A335" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B335" s="10"/>
+      <c r="C335" s="10"/>
+      <c r="D335" s="10"/>
+      <c r="E335" s="10"/>
+      <c r="F335" s="10"/>
+      <c r="G335" s="10"/>
+      <c r="L335" s="13"/>
+      <c r="M335" s="13"/>
+      <c r="N335" s="13"/>
+      <c r="O335" s="13"/>
+      <c r="P335" s="13"/>
+    </row>
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A336" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B336" s="10"/>
+      <c r="C336" s="10"/>
+      <c r="D336" s="10"/>
+      <c r="E336" s="10"/>
+      <c r="F336" s="10"/>
+      <c r="G336" s="10"/>
+      <c r="L336" s="13"/>
+      <c r="M336" s="13"/>
+      <c r="N336" s="13"/>
+      <c r="O336" s="13"/>
+      <c r="P336" s="13"/>
+    </row>
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A337" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B337" s="10"/>
+      <c r="C337" s="10"/>
+      <c r="D337" s="10"/>
+      <c r="E337" s="10"/>
+      <c r="F337" s="10"/>
+      <c r="G337" s="10"/>
+      <c r="L337" s="13"/>
+      <c r="M337" s="13"/>
+      <c r="N337" s="13"/>
+      <c r="O337" s="13"/>
+      <c r="P337" s="13"/>
+    </row>
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A338" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B338" s="10"/>
+      <c r="C338" s="10"/>
+      <c r="D338" s="10"/>
+      <c r="E338" s="10"/>
+      <c r="F338" s="10"/>
+      <c r="G338" s="10"/>
+      <c r="L338" s="13"/>
+      <c r="M338" s="13"/>
+      <c r="N338" s="14"/>
+      <c r="O338" s="13"/>
+      <c r="P338" s="13"/>
+    </row>
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A339" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B339" s="10"/>
+      <c r="C339" s="10"/>
+      <c r="D339" s="10"/>
+      <c r="E339" s="10"/>
+      <c r="F339" s="10"/>
+      <c r="G339" s="10"/>
+      <c r="L339" s="13"/>
+      <c r="M339" s="13"/>
+      <c r="N339" s="13"/>
+      <c r="O339" s="13"/>
+      <c r="P339" s="13"/>
+    </row>
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A340" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B340" s="10"/>
+      <c r="C340" s="10"/>
+      <c r="D340" s="10"/>
+      <c r="E340" s="10"/>
+      <c r="F340" s="10"/>
+      <c r="G340" s="10"/>
+      <c r="L340" s="13"/>
+      <c r="M340" s="13"/>
+      <c r="N340" s="13"/>
+      <c r="O340" s="13"/>
+      <c r="P340" s="13"/>
+    </row>
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A341" s="10"/>
+      <c r="B341" s="10"/>
+      <c r="C341" s="10"/>
+      <c r="D341" s="10"/>
+      <c r="E341" s="10"/>
+      <c r="F341" s="10"/>
+      <c r="G341" s="10"/>
+      <c r="L341" s="13"/>
+      <c r="M341" s="13"/>
+      <c r="N341" s="13"/>
+      <c r="O341" s="13"/>
+      <c r="P341" s="13"/>
+    </row>
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A342" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B342" s="10"/>
+      <c r="C342" s="10"/>
+      <c r="D342" s="10"/>
+      <c r="E342" s="10"/>
+      <c r="F342" s="10"/>
+      <c r="G342" s="10"/>
+      <c r="L342" s="13"/>
+      <c r="M342" s="13"/>
+      <c r="N342" s="13"/>
+      <c r="O342" s="13"/>
+      <c r="P342" s="13"/>
+    </row>
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A343" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B343" s="10"/>
+      <c r="C343" s="10"/>
+      <c r="D343" s="10"/>
+      <c r="E343" s="10"/>
+      <c r="F343" s="10"/>
+      <c r="G343" s="10"/>
+      <c r="L343" s="13"/>
+      <c r="M343" s="13"/>
+      <c r="N343" s="13"/>
+      <c r="O343" s="13"/>
+      <c r="P343" s="13"/>
+    </row>
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A344" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B344" s="10"/>
+      <c r="C344" s="10"/>
+      <c r="D344" s="10"/>
+      <c r="E344" s="10"/>
+      <c r="F344" s="10"/>
+      <c r="G344" s="10"/>
+      <c r="L344" s="13"/>
+      <c r="M344" s="13"/>
+      <c r="N344" s="13"/>
+      <c r="O344" s="13"/>
+      <c r="P344" s="13"/>
+    </row>
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A345" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B345" s="10"/>
+      <c r="C345" s="10"/>
+      <c r="D345" s="10"/>
+      <c r="E345" s="10"/>
+      <c r="F345" s="10"/>
+      <c r="G345" s="10"/>
+      <c r="L345" s="13"/>
+      <c r="M345" s="13"/>
+      <c r="N345" s="13"/>
+      <c r="O345" s="13"/>
+      <c r="P345" s="13"/>
+    </row>
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A346" s="10"/>
+      <c r="B346" s="10"/>
+      <c r="C346" s="10"/>
+      <c r="D346" s="10"/>
+      <c r="E346" s="10"/>
+      <c r="F346" s="10"/>
+      <c r="G346" s="10"/>
+      <c r="L346" s="13"/>
+      <c r="M346" s="13"/>
+      <c r="N346" s="13"/>
+      <c r="O346" s="13"/>
+      <c r="P346" s="13"/>
+    </row>
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A347" s="10"/>
+      <c r="B347" s="10"/>
+      <c r="C347" s="10"/>
+      <c r="D347" s="10"/>
+      <c r="E347" s="10"/>
+      <c r="F347" s="10"/>
+      <c r="G347" s="10"/>
+      <c r="L347" s="13"/>
+      <c r="M347" s="13"/>
+      <c r="N347" s="13"/>
+      <c r="O347" s="13"/>
+      <c r="P347" s="13"/>
+    </row>
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A348" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B348" s="10"/>
+      <c r="C348" s="10"/>
+      <c r="D348" s="10"/>
+      <c r="E348" s="10"/>
+      <c r="F348" s="10"/>
+      <c r="G348" s="10"/>
+    </row>
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A349" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B349" s="10"/>
+      <c r="C349" s="10"/>
+      <c r="D349" s="10"/>
+      <c r="E349" s="10"/>
+      <c r="F349" s="10"/>
+      <c r="G349" s="10"/>
+    </row>
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A350" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B350" s="10"/>
+      <c r="C350" s="10"/>
+      <c r="D350" s="10"/>
+      <c r="E350" s="10"/>
+      <c r="F350" s="10"/>
+      <c r="G350" s="10"/>
+    </row>
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A351" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B351" s="10"/>
+      <c r="C351" s="10"/>
+      <c r="D351" s="10"/>
+      <c r="E351" s="10"/>
+      <c r="F351" s="10"/>
+      <c r="G351" s="10"/>
+    </row>
+    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A352" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B352" s="10"/>
+      <c r="C352" s="10"/>
+      <c r="D352" s="10"/>
+      <c r="E352" s="10"/>
+      <c r="F352" s="10"/>
+      <c r="G352" s="10"/>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A353" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B353" s="10"/>
+      <c r="C353" s="10"/>
+      <c r="D353" s="10"/>
+      <c r="E353" s="10"/>
+      <c r="F353" s="10"/>
+      <c r="G353" s="10"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A354" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B354" s="10"/>
+      <c r="C354" s="10"/>
+      <c r="D354" s="10"/>
+      <c r="E354" s="10"/>
+      <c r="F354" s="10"/>
+      <c r="G354" s="10"/>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A355" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B355" s="10"/>
+      <c r="C355" s="10"/>
+      <c r="D355" s="10"/>
+      <c r="E355" s="10"/>
+      <c r="F355" s="10"/>
+      <c r="G355" s="10"/>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A356" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B356" s="10"/>
+      <c r="C356" s="10"/>
+      <c r="D356" s="10"/>
+      <c r="E356" s="10"/>
+      <c r="F356" s="10"/>
+      <c r="G356" s="10"/>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A357" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B357" s="10"/>
+      <c r="C357" s="10"/>
+      <c r="D357" s="10"/>
+      <c r="E357" s="10"/>
+      <c r="F357" s="10"/>
+      <c r="G357" s="10"/>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A358" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B358" s="10"/>
+      <c r="C358" s="10"/>
+      <c r="D358" s="10"/>
+      <c r="E358" s="10"/>
+      <c r="F358" s="10"/>
+      <c r="G358" s="10"/>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A359" s="10"/>
+      <c r="B359" s="10"/>
+      <c r="C359" s="10"/>
+      <c r="D359" s="10"/>
+      <c r="E359" s="10"/>
+      <c r="F359" s="10"/>
+      <c r="G359" s="10"/>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A360" s="10"/>
+      <c r="B360" s="10"/>
+      <c r="C360" s="10"/>
+      <c r="D360" s="10"/>
+      <c r="E360" s="10"/>
+      <c r="F360" s="10"/>
+      <c r="G360" s="10"/>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A361" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B361" s="10"/>
+      <c r="C361" s="10"/>
+      <c r="D361" s="10"/>
+      <c r="E361" s="10"/>
+      <c r="F361" s="10"/>
+      <c r="G361" s="10"/>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A362" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B362" s="10"/>
+      <c r="C362" s="10"/>
+      <c r="D362" s="10"/>
+      <c r="E362" s="10"/>
+      <c r="F362" s="10"/>
+      <c r="G362" s="10"/>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B363" s="10"/>
+      <c r="C363" s="10"/>
+      <c r="D363" s="10"/>
+      <c r="E363" s="10"/>
+      <c r="F363" s="10"/>
+      <c r="G363" s="10"/>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A364" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B364" s="10"/>
+      <c r="C364" s="10"/>
+      <c r="D364" s="10"/>
+      <c r="E364" s="10"/>
+      <c r="F364" s="10"/>
+      <c r="G364" s="10"/>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A365" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B365" s="10"/>
+      <c r="C365" s="10"/>
+      <c r="D365" s="10"/>
+      <c r="E365" s="10"/>
+      <c r="F365" s="10"/>
+      <c r="G365" s="10"/>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A366" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B366" s="10"/>
+      <c r="C366" s="10"/>
+      <c r="D366" s="10"/>
+      <c r="E366" s="10"/>
+      <c r="F366" s="10"/>
+      <c r="G366" s="10"/>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B367" s="10"/>
+      <c r="C367" s="10"/>
+      <c r="D367" s="10"/>
+      <c r="E367" s="10"/>
+      <c r="F367" s="10"/>
+      <c r="G367" s="10"/>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B368" s="10"/>
+      <c r="C368" s="10"/>
+      <c r="D368" s="10"/>
+      <c r="E368" s="10"/>
+      <c r="F368" s="10"/>
+      <c r="G368" s="10"/>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A369" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B369" s="10"/>
+      <c r="C369" s="10"/>
+      <c r="D369" s="10"/>
+      <c r="E369" s="10"/>
+      <c r="F369" s="10"/>
+      <c r="G369" s="10"/>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A370" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B370" s="10"/>
+      <c r="C370" s="10"/>
+      <c r="D370" s="10"/>
+      <c r="E370" s="10"/>
+      <c r="F370" s="10"/>
+      <c r="G370" s="10"/>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A371" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B371" s="10"/>
+      <c r="C371" s="10"/>
+      <c r="D371" s="10"/>
+      <c r="E371" s="10"/>
+      <c r="F371" s="10"/>
+      <c r="G371" s="10"/>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A372" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B372" s="10"/>
+      <c r="C372" s="10"/>
+      <c r="D372" s="10"/>
+      <c r="E372" s="10"/>
+      <c r="F372" s="10"/>
+      <c r="G372" s="10"/>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A373" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B373" s="10"/>
+      <c r="C373" s="10"/>
+      <c r="D373" s="10"/>
+      <c r="E373" s="10"/>
+      <c r="F373" s="10"/>
+      <c r="G373" s="10"/>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A374" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B374" s="10"/>
+      <c r="C374" s="10"/>
+      <c r="D374" s="10"/>
+      <c r="E374" s="10"/>
+      <c r="F374" s="10"/>
+      <c r="G374" s="10"/>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A375" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B375" s="10"/>
+      <c r="C375" s="10"/>
+      <c r="D375" s="10"/>
+      <c r="E375" s="10"/>
+      <c r="F375" s="10"/>
+      <c r="G375" s="10"/>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A376" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B376" s="10"/>
+      <c r="C376" s="10"/>
+      <c r="D376" s="10"/>
+      <c r="E376" s="10"/>
+      <c r="F376" s="10"/>
+      <c r="G376" s="10"/>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A377" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B377" s="10"/>
+      <c r="C377" s="10"/>
+      <c r="D377" s="10"/>
+      <c r="E377" s="10"/>
+      <c r="F377" s="10"/>
+      <c r="G377" s="10"/>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A378" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B378" s="10"/>
+      <c r="C378" s="10"/>
+      <c r="D378" s="10"/>
+      <c r="E378" s="10"/>
+      <c r="F378" s="10"/>
+      <c r="G378" s="10"/>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A379" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B379" s="10"/>
+      <c r="C379" s="10"/>
+      <c r="D379" s="10"/>
+      <c r="E379" s="10"/>
+      <c r="F379" s="10"/>
+      <c r="G379" s="10"/>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B383" s="6"/>
+      <c r="C383" s="6"/>
+      <c r="D383" s="6"/>
+      <c r="E383" s="6"/>
+      <c r="F383" s="6"/>
+      <c r="G383" s="6"/>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B384" s="3"/>
+      <c r="C384" s="3"/>
+      <c r="D384" s="3"/>
+      <c r="E384" s="3"/>
+      <c r="F384" s="3"/>
+      <c r="G384" s="3"/>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B385" s="3"/>
+      <c r="C385" s="3"/>
+      <c r="D385" s="3"/>
+      <c r="E385" s="3"/>
+      <c r="F385" s="3"/>
+      <c r="G385" s="3"/>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B386" s="3"/>
+      <c r="C386" s="3"/>
+      <c r="D386" s="3"/>
+      <c r="E386" s="3"/>
+      <c r="F386" s="3"/>
+      <c r="G386" s="3"/>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A387" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B387" s="3"/>
+      <c r="C387" s="3"/>
+      <c r="D387" s="3"/>
+      <c r="E387" s="3"/>
+      <c r="F387" s="3"/>
+      <c r="G387" s="3"/>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A388" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B388" s="3"/>
+      <c r="C388" s="3"/>
+      <c r="D388" s="3"/>
+      <c r="E388" s="3"/>
+      <c r="F388" s="3"/>
+      <c r="G388" s="3"/>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A389" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B389" s="3"/>
+      <c r="C389" s="3"/>
+      <c r="D389" s="3"/>
+      <c r="E389" s="3"/>
+      <c r="F389" s="3"/>
+      <c r="G389" s="3"/>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A390" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B390" s="3"/>
+      <c r="C390" s="3"/>
+      <c r="D390" s="3"/>
+      <c r="E390" s="3"/>
+      <c r="F390" s="3"/>
+      <c r="G390" s="3"/>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B391" s="3"/>
+      <c r="C391" s="3"/>
+      <c r="D391" s="3"/>
+      <c r="E391" s="3"/>
+      <c r="F391" s="3"/>
+      <c r="G391" s="3"/>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B392" s="3"/>
+      <c r="C392" s="3"/>
+      <c r="D392" s="3"/>
+      <c r="E392" s="3"/>
+      <c r="F392" s="3"/>
+      <c r="G392" s="3"/>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A393" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B393" s="3"/>
+      <c r="C393" s="3"/>
+      <c r="D393" s="3"/>
+      <c r="E393" s="3"/>
+      <c r="F393" s="3"/>
+      <c r="G393" s="3"/>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A394" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B394" s="3"/>
+      <c r="C394" s="3"/>
+      <c r="D394" s="3"/>
+      <c r="E394" s="3"/>
+      <c r="F394" s="3"/>
+      <c r="G394" s="3"/>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A395" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B395" s="3"/>
+      <c r="C395" s="3"/>
+      <c r="D395" s="3"/>
+      <c r="E395" s="3"/>
+      <c r="F395" s="3"/>
+      <c r="G395" s="3"/>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A396" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B396" s="3"/>
+      <c r="C396" s="3"/>
+      <c r="D396" s="3"/>
+      <c r="E396" s="3"/>
+      <c r="F396" s="3"/>
+      <c r="G396" s="3"/>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B397" s="3"/>
+      <c r="C397" s="3"/>
+      <c r="D397" s="3"/>
+      <c r="E397" s="3"/>
+      <c r="F397" s="3"/>
+      <c r="G397" s="3"/>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A398" s="3"/>
+      <c r="B398" s="3"/>
+      <c r="C398" s="3"/>
+      <c r="D398" s="3"/>
+      <c r="E398" s="3"/>
+      <c r="F398" s="3"/>
+      <c r="G398" s="3"/>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B399" s="3"/>
+      <c r="C399" s="3"/>
+      <c r="D399" s="3"/>
+      <c r="E399" s="3"/>
+      <c r="F399" s="3"/>
+      <c r="G399" s="3"/>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A400" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B400" s="3"/>
+      <c r="C400" s="3"/>
+      <c r="D400" s="3"/>
+      <c r="E400" s="3"/>
+      <c r="F400" s="3"/>
+      <c r="G400" s="3"/>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A401" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B401" s="3"/>
+      <c r="C401" s="3"/>
+      <c r="D401" s="3"/>
+      <c r="E401" s="3"/>
+      <c r="F401" s="3"/>
+      <c r="G401" s="3"/>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A402" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B402" s="3"/>
+      <c r="C402" s="3"/>
+      <c r="D402" s="3"/>
+      <c r="E402" s="3"/>
+      <c r="F402" s="3"/>
+      <c r="G402" s="3"/>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A403" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B403" s="3"/>
+      <c r="C403" s="3"/>
+      <c r="D403" s="3"/>
+      <c r="E403" s="3"/>
+      <c r="F403" s="3"/>
+      <c r="G403" s="3"/>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A404" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B404" s="3"/>
+      <c r="C404" s="3"/>
+      <c r="D404" s="3"/>
+      <c r="E404" s="3"/>
+      <c r="F404" s="3"/>
+      <c r="G404" s="3"/>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A405" s="3"/>
+      <c r="B405" s="3"/>
+      <c r="C405" s="3"/>
+      <c r="D405" s="3"/>
+      <c r="E405" s="3"/>
+      <c r="F405" s="3"/>
+      <c r="G405" s="3"/>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A406" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B406" s="3"/>
+      <c r="C406" s="3"/>
+      <c r="D406" s="3"/>
+      <c r="E406" s="3"/>
+      <c r="F406" s="3"/>
+      <c r="G406" s="3"/>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A407" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B407" s="3"/>
+      <c r="C407" s="3"/>
+      <c r="D407" s="3"/>
+      <c r="E407" s="3"/>
+      <c r="F407" s="3"/>
+      <c r="G407" s="3"/>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B408" s="3"/>
+      <c r="C408" s="3"/>
+      <c r="D408" s="3"/>
+      <c r="E408" s="3"/>
+      <c r="F408" s="3"/>
+      <c r="G408" s="3"/>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A409" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B409" s="3"/>
+      <c r="C409" s="3"/>
+      <c r="D409" s="3"/>
+      <c r="E409" s="3"/>
+      <c r="F409" s="3"/>
+      <c r="G409" s="3"/>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A410" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B410" s="3"/>
+      <c r="C410" s="3"/>
+      <c r="D410" s="3"/>
+      <c r="E410" s="3"/>
+      <c r="F410" s="3"/>
+      <c r="G410" s="3"/>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A411" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B411" s="3"/>
+      <c r="C411" s="3"/>
+      <c r="D411" s="3"/>
+      <c r="E411" s="3"/>
+      <c r="F411" s="3"/>
+      <c r="G411" s="3"/>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B412" s="3"/>
+      <c r="C412" s="3"/>
+      <c r="D412" s="3"/>
+      <c r="E412" s="3"/>
+      <c r="F412" s="3"/>
+      <c r="G412" s="3"/>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A413" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B413" s="3"/>
+      <c r="C413" s="3"/>
+      <c r="D413" s="3"/>
+      <c r="E413" s="3"/>
+      <c r="F413" s="3"/>
+      <c r="G413" s="3"/>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A414" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B414" s="3"/>
+      <c r="C414" s="3"/>
+      <c r="D414" s="3"/>
+      <c r="E414" s="3"/>
+      <c r="F414" s="3"/>
+      <c r="G414" s="3"/>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A415" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B415" s="3"/>
+      <c r="C415" s="3"/>
+      <c r="D415" s="3"/>
+      <c r="E415" s="3"/>
+      <c r="F415" s="3"/>
+      <c r="G415" s="3"/>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A416" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B416" s="3"/>
+      <c r="C416" s="3"/>
+      <c r="D416" s="3"/>
+      <c r="E416" s="3"/>
+      <c r="F416" s="3"/>
+      <c r="G416" s="3"/>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A417" s="3"/>
+      <c r="B417" s="3"/>
+      <c r="C417" s="3"/>
+      <c r="D417" s="3"/>
+      <c r="E417" s="3"/>
+      <c r="F417" s="3"/>
+      <c r="G417" s="3"/>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A418" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B418" s="3"/>
+      <c r="C418" s="3"/>
+      <c r="D418" s="3"/>
+      <c r="E418" s="3"/>
+      <c r="F418" s="3"/>
+      <c r="G418" s="3"/>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A419" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B419" s="3"/>
+      <c r="C419" s="3"/>
+      <c r="D419" s="3"/>
+      <c r="E419" s="3"/>
+      <c r="F419" s="3"/>
+      <c r="G419" s="3"/>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A420" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B420" s="3"/>
+      <c r="C420" s="3"/>
+      <c r="D420" s="3"/>
+      <c r="E420" s="3"/>
+      <c r="F420" s="3"/>
+      <c r="G420" s="3"/>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A421" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B421" s="3"/>
+      <c r="C421" s="3"/>
+      <c r="D421" s="3"/>
+      <c r="E421" s="3"/>
+      <c r="F421" s="3"/>
+      <c r="G421" s="3"/>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A422" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B422" s="3"/>
+      <c r="C422" s="3"/>
+      <c r="D422" s="3"/>
+      <c r="E422" s="3"/>
+      <c r="F422" s="3"/>
+      <c r="G422" s="3"/>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A423" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B423" s="3"/>
+      <c r="C423" s="3"/>
+      <c r="D423" s="3"/>
+      <c r="E423" s="3"/>
+      <c r="F423" s="3"/>
+      <c r="G423" s="3"/>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A424" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B424" s="3"/>
+      <c r="C424" s="3"/>
+      <c r="D424" s="3"/>
+      <c r="E424" s="3"/>
+      <c r="F424" s="3"/>
+      <c r="G424" s="3"/>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A425" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B425" s="3"/>
+      <c r="C425" s="3"/>
+      <c r="D425" s="3"/>
+      <c r="E425" s="3"/>
+      <c r="F425" s="3"/>
+      <c r="G425" s="3"/>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A426" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B426" s="3"/>
+      <c r="C426" s="3"/>
+      <c r="D426" s="3"/>
+      <c r="E426" s="3"/>
+      <c r="F426" s="3"/>
+      <c r="G426" s="3"/>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A427" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B427" s="3"/>
+      <c r="C427" s="3"/>
+      <c r="D427" s="3"/>
+      <c r="E427" s="3"/>
+      <c r="F427" s="3"/>
+      <c r="G427" s="3"/>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A428" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B428" s="3"/>
+      <c r="C428" s="3"/>
+      <c r="D428" s="3"/>
+      <c r="E428" s="3"/>
+      <c r="F428" s="3"/>
+      <c r="G428" s="3"/>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A429" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B429" s="3"/>
+      <c r="C429" s="3"/>
+      <c r="D429" s="3"/>
+      <c r="E429" s="3"/>
+      <c r="F429" s="3"/>
+      <c r="G429" s="3"/>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A430" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B430" s="3"/>
+      <c r="C430" s="3"/>
+      <c r="D430" s="3"/>
+      <c r="E430" s="3"/>
+      <c r="F430" s="3"/>
+      <c r="G430" s="3"/>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A431" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B431" s="3"/>
+      <c r="C431" s="3"/>
+      <c r="D431" s="3"/>
+      <c r="E431" s="3"/>
+      <c r="F431" s="3"/>
+      <c r="G431" s="3"/>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A432" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B432" s="3"/>
+      <c r="C432" s="3"/>
+      <c r="D432" s="3"/>
+      <c r="E432" s="3"/>
+      <c r="F432" s="3"/>
+      <c r="G432" s="3"/>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A433" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B433" s="3"/>
+      <c r="C433" s="3"/>
+      <c r="D433" s="3"/>
+      <c r="E433" s="3"/>
+      <c r="F433" s="3"/>
+      <c r="G433" s="3"/>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A434" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B434" s="3"/>
+      <c r="C434" s="3"/>
+      <c r="D434" s="3"/>
+      <c r="E434" s="3"/>
+      <c r="F434" s="3"/>
+      <c r="G434" s="3"/>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A435" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B435" s="3"/>
+      <c r="C435" s="3"/>
+      <c r="D435" s="3"/>
+      <c r="E435" s="3"/>
+      <c r="F435" s="3"/>
+      <c r="G435" s="3"/>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A436" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B436" s="3"/>
+      <c r="C436" s="3"/>
+      <c r="D436" s="3"/>
+      <c r="E436" s="3"/>
+      <c r="F436" s="3"/>
+      <c r="G436" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A258:G258"/>
+    <mergeCell ref="A259:C259"/>
+    <mergeCell ref="A284:C284"/>
+    <mergeCell ref="A383:G383"/>
     <mergeCell ref="A172:G172"/>
+    <mergeCell ref="A218:G218"/>
     <mergeCell ref="A37:G37"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A1:G1"/>

</xml_diff>

<commit_message>
Se sube backup y metadata de hasura
</commit_message>
<xml_diff>
--- a/ListadoQuerys.xlsx
+++ b/ListadoQuerys.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProyectoPesLac\peslac-back\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto PESLAC\peslac-back\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F16AB-AEDA-4F71-8A80-6D702A5A20A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7113A75-7057-49B6-A06F-F794DEE783D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5AE78F90-65AD-4FFA-A2BC-D2300784A877}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="194">
   <si>
     <t>query ConsultaProductos {</t>
   </si>
@@ -566,6 +566,57 @@
   </si>
   <si>
     <t xml:space="preserve">  insert_historial_devoluciones_salidas_productos_one(object: {id_producto: $id_producto, id_tipo_operacion: 1, comentario: "Salida de producto por compra", cantidad: $cantidad}) {</t>
+  </si>
+  <si>
+    <t>query ConsultarHistoricoComprasGeneral {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  compras(order_by: {id: asc}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        total</t>
+  </si>
+  <si>
+    <t>Historial Compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  vis_detalle_compras {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    id_venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    linea_producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    proveedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    total</t>
+  </si>
+  <si>
+    <t>query ConsultarHistoricoComprasDetallado {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  compras(where: {id: {_eq: $idCompra}}) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        valor_impuesto</t>
+  </si>
+  <si>
+    <t>query ConsultarDetalleCompra($idCompra: Int = 1) {</t>
+  </si>
+  <si>
+    <t>Consulta el detalle de la compra filtrando por el id</t>
+  </si>
+  <si>
+    <t>Consulta el historico de compras detallado</t>
+  </si>
+  <si>
+    <t>Consulta el historico de compras general</t>
   </si>
 </sst>
 </file>
@@ -639,20 +690,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,6 +706,20 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,24 +1034,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E99040-D82E-45BB-95AB-EA9D37042862}">
-  <dimension ref="A1:P436"/>
+  <dimension ref="A1:P520"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
-      <selection activeCell="A414" sqref="A414"/>
+    <sheetView tabSelected="1" topLeftCell="A491" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G449" sqref="G449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1363,15 +1422,15 @@
       <c r="G35" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -1542,15 +1601,15 @@
       <c r="G53" s="1"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -2027,15 +2086,15 @@
       <c r="G102" s="2"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
@@ -2362,15 +2421,15 @@
       <c r="G135" s="3"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B140" s="6"/>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
@@ -2664,15 +2723,15 @@
       <c r="G167" s="4"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A172" s="6" t="s">
+      <c r="A172" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
-      <c r="G172" s="6"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
@@ -3144,18 +3203,18 @@
       <c r="G215" s="1"/>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A218" s="6" t="s">
+      <c r="A218" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B218" s="6"/>
-      <c r="C218" s="6"/>
-      <c r="D218" s="6"/>
-      <c r="E218" s="6"/>
-      <c r="F218" s="6"/>
-      <c r="G218" s="6"/>
+      <c r="B218" s="13"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="13"/>
+      <c r="G218" s="13"/>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219" s="7" t="s">
+      <c r="A219" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B219" s="3"/>
@@ -3221,7 +3280,7 @@
       <c r="G224" s="3"/>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" s="7" t="s">
+      <c r="A225" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B225" s="3"/>
@@ -3318,7 +3377,7 @@
       <c r="G233" s="3"/>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A234" s="7" t="s">
+      <c r="A234" s="6" t="s">
         <v>148</v>
       </c>
       <c r="B234" s="3"/>
@@ -3411,7 +3470,7 @@
       <c r="G242" s="3"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243" s="7" t="s">
+      <c r="A243" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B243" s="3"/>
@@ -3541,1419 +3600,1419 @@
       <c r="G254" s="3"/>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A258" s="6" t="s">
+      <c r="A258" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B258" s="6"/>
-      <c r="C258" s="6"/>
-      <c r="D258" s="6"/>
-      <c r="E258" s="6"/>
-      <c r="F258" s="6"/>
-      <c r="G258" s="6"/>
+      <c r="B258" s="13"/>
+      <c r="C258" s="13"/>
+      <c r="D258" s="13"/>
+      <c r="E258" s="13"/>
+      <c r="F258" s="13"/>
+      <c r="G258" s="13"/>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A259" s="8" t="s">
+      <c r="A259" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B259" s="8"/>
-      <c r="C259" s="8"/>
-      <c r="D259" s="9"/>
-      <c r="E259" s="9"/>
-      <c r="F259" s="9"/>
-      <c r="G259" s="9"/>
+      <c r="B259" s="14"/>
+      <c r="C259" s="14"/>
+      <c r="D259" s="7"/>
+      <c r="E259" s="7"/>
+      <c r="F259" s="7"/>
+      <c r="G259" s="7"/>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A260" s="10" t="s">
+      <c r="A260" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B260" s="10"/>
-      <c r="C260" s="10"/>
-      <c r="D260" s="10"/>
-      <c r="E260" s="10"/>
-      <c r="F260" s="10"/>
-      <c r="G260" s="10"/>
+      <c r="B260" s="8"/>
+      <c r="C260" s="8"/>
+      <c r="D260" s="8"/>
+      <c r="E260" s="8"/>
+      <c r="F260" s="8"/>
+      <c r="G260" s="8"/>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="10" t="s">
+      <c r="A261" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B261" s="10"/>
-      <c r="C261" s="10"/>
-      <c r="D261" s="10"/>
-      <c r="E261" s="10"/>
-      <c r="F261" s="10"/>
-      <c r="G261" s="10"/>
+      <c r="B261" s="8"/>
+      <c r="C261" s="8"/>
+      <c r="D261" s="8"/>
+      <c r="E261" s="8"/>
+      <c r="F261" s="8"/>
+      <c r="G261" s="8"/>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="10" t="s">
+      <c r="A262" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B262" s="10"/>
-      <c r="C262" s="10"/>
-      <c r="D262" s="10"/>
-      <c r="E262" s="10"/>
-      <c r="F262" s="10"/>
-      <c r="G262" s="10"/>
+      <c r="B262" s="8"/>
+      <c r="C262" s="8"/>
+      <c r="D262" s="8"/>
+      <c r="E262" s="8"/>
+      <c r="F262" s="8"/>
+      <c r="G262" s="8"/>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A263" s="10" t="s">
+      <c r="A263" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B263" s="10"/>
-      <c r="C263" s="10"/>
-      <c r="D263" s="10"/>
-      <c r="E263" s="10"/>
-      <c r="F263" s="10"/>
-      <c r="G263" s="10"/>
+      <c r="B263" s="8"/>
+      <c r="C263" s="8"/>
+      <c r="D263" s="8"/>
+      <c r="E263" s="8"/>
+      <c r="F263" s="8"/>
+      <c r="G263" s="8"/>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A264" s="10" t="s">
+      <c r="A264" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B264" s="10"/>
-      <c r="C264" s="10"/>
-      <c r="D264" s="10"/>
-      <c r="E264" s="10"/>
-      <c r="F264" s="10"/>
-      <c r="G264" s="10"/>
+      <c r="B264" s="8"/>
+      <c r="C264" s="8"/>
+      <c r="D264" s="8"/>
+      <c r="E264" s="8"/>
+      <c r="F264" s="8"/>
+      <c r="G264" s="8"/>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" s="10" t="s">
+      <c r="A265" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B265" s="10"/>
-      <c r="C265" s="10"/>
-      <c r="D265" s="10"/>
-      <c r="E265" s="10"/>
-      <c r="F265" s="10"/>
-      <c r="G265" s="10"/>
+      <c r="B265" s="8"/>
+      <c r="C265" s="8"/>
+      <c r="D265" s="8"/>
+      <c r="E265" s="8"/>
+      <c r="F265" s="8"/>
+      <c r="G265" s="8"/>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A266" s="10" t="s">
+      <c r="A266" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B266" s="10"/>
-      <c r="C266" s="10"/>
-      <c r="D266" s="10"/>
-      <c r="E266" s="10"/>
-      <c r="F266" s="10"/>
-      <c r="G266" s="10"/>
+      <c r="B266" s="8"/>
+      <c r="C266" s="8"/>
+      <c r="D266" s="8"/>
+      <c r="E266" s="8"/>
+      <c r="F266" s="8"/>
+      <c r="G266" s="8"/>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A267" s="10" t="s">
+      <c r="A267" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B267" s="10"/>
-      <c r="C267" s="10"/>
-      <c r="D267" s="10"/>
-      <c r="E267" s="10"/>
-      <c r="F267" s="10"/>
-      <c r="G267" s="10"/>
+      <c r="B267" s="8"/>
+      <c r="C267" s="8"/>
+      <c r="D267" s="8"/>
+      <c r="E267" s="8"/>
+      <c r="F267" s="8"/>
+      <c r="G267" s="8"/>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A268" s="10" t="s">
+      <c r="A268" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B268" s="10"/>
-      <c r="C268" s="10"/>
-      <c r="D268" s="10"/>
-      <c r="E268" s="10"/>
-      <c r="F268" s="10"/>
-      <c r="G268" s="10"/>
+      <c r="B268" s="8"/>
+      <c r="C268" s="8"/>
+      <c r="D268" s="8"/>
+      <c r="E268" s="8"/>
+      <c r="F268" s="8"/>
+      <c r="G268" s="8"/>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="10" t="s">
+      <c r="A269" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B269" s="10"/>
-      <c r="C269" s="10"/>
-      <c r="D269" s="10"/>
-      <c r="E269" s="10"/>
-      <c r="F269" s="10"/>
-      <c r="G269" s="10"/>
+      <c r="B269" s="8"/>
+      <c r="C269" s="8"/>
+      <c r="D269" s="8"/>
+      <c r="E269" s="8"/>
+      <c r="F269" s="8"/>
+      <c r="G269" s="8"/>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" s="10" t="s">
+      <c r="A270" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B270" s="10"/>
-      <c r="C270" s="10"/>
-      <c r="D270" s="10"/>
-      <c r="E270" s="10"/>
-      <c r="F270" s="10"/>
-      <c r="G270" s="10"/>
+      <c r="B270" s="8"/>
+      <c r="C270" s="8"/>
+      <c r="D270" s="8"/>
+      <c r="E270" s="8"/>
+      <c r="F270" s="8"/>
+      <c r="G270" s="8"/>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A271" s="10" t="s">
+      <c r="A271" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B271" s="10"/>
-      <c r="C271" s="10"/>
-      <c r="D271" s="10"/>
-      <c r="E271" s="10"/>
-      <c r="F271" s="10"/>
-      <c r="G271" s="10"/>
+      <c r="B271" s="8"/>
+      <c r="C271" s="8"/>
+      <c r="D271" s="8"/>
+      <c r="E271" s="8"/>
+      <c r="F271" s="8"/>
+      <c r="G271" s="8"/>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272" s="10" t="s">
+      <c r="A272" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B272" s="10"/>
-      <c r="C272" s="10"/>
-      <c r="D272" s="10"/>
-      <c r="E272" s="10"/>
-      <c r="F272" s="10"/>
-      <c r="G272" s="10"/>
+      <c r="B272" s="8"/>
+      <c r="C272" s="8"/>
+      <c r="D272" s="8"/>
+      <c r="E272" s="8"/>
+      <c r="F272" s="8"/>
+      <c r="G272" s="8"/>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273" s="10" t="s">
+      <c r="A273" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B273" s="10"/>
-      <c r="C273" s="10"/>
-      <c r="D273" s="10"/>
-      <c r="E273" s="10"/>
-      <c r="F273" s="10"/>
-      <c r="G273" s="10"/>
+      <c r="B273" s="8"/>
+      <c r="C273" s="8"/>
+      <c r="D273" s="8"/>
+      <c r="E273" s="8"/>
+      <c r="F273" s="8"/>
+      <c r="G273" s="8"/>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274" s="10" t="s">
+      <c r="A274" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B274" s="10"/>
-      <c r="C274" s="10"/>
-      <c r="D274" s="10"/>
-      <c r="E274" s="10"/>
-      <c r="F274" s="10"/>
-      <c r="G274" s="10"/>
+      <c r="B274" s="8"/>
+      <c r="C274" s="8"/>
+      <c r="D274" s="8"/>
+      <c r="E274" s="8"/>
+      <c r="F274" s="8"/>
+      <c r="G274" s="8"/>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275" s="10" t="s">
+      <c r="A275" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B275" s="10"/>
-      <c r="C275" s="10"/>
-      <c r="D275" s="10"/>
-      <c r="E275" s="10"/>
-      <c r="F275" s="10"/>
-      <c r="G275" s="10"/>
+      <c r="B275" s="8"/>
+      <c r="C275" s="8"/>
+      <c r="D275" s="8"/>
+      <c r="E275" s="8"/>
+      <c r="F275" s="8"/>
+      <c r="G275" s="8"/>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A276" s="10" t="s">
+      <c r="A276" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B276" s="10"/>
-      <c r="C276" s="10"/>
-      <c r="D276" s="10"/>
-      <c r="E276" s="10"/>
-      <c r="F276" s="10"/>
-      <c r="G276" s="10"/>
+      <c r="B276" s="8"/>
+      <c r="C276" s="8"/>
+      <c r="D276" s="8"/>
+      <c r="E276" s="8"/>
+      <c r="F276" s="8"/>
+      <c r="G276" s="8"/>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="10" t="s">
+      <c r="A277" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B277" s="10"/>
-      <c r="C277" s="10"/>
-      <c r="D277" s="10"/>
-      <c r="E277" s="10"/>
-      <c r="F277" s="10"/>
-      <c r="G277" s="10"/>
+      <c r="B277" s="8"/>
+      <c r="C277" s="8"/>
+      <c r="D277" s="8"/>
+      <c r="E277" s="8"/>
+      <c r="F277" s="8"/>
+      <c r="G277" s="8"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="10" t="s">
+      <c r="A278" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B278" s="10"/>
-      <c r="C278" s="10"/>
-      <c r="D278" s="10"/>
-      <c r="E278" s="10"/>
-      <c r="F278" s="10"/>
-      <c r="G278" s="10"/>
+      <c r="B278" s="8"/>
+      <c r="C278" s="8"/>
+      <c r="D278" s="8"/>
+      <c r="E278" s="8"/>
+      <c r="F278" s="8"/>
+      <c r="G278" s="8"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" s="10" t="s">
+      <c r="A279" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B279" s="10"/>
-      <c r="C279" s="10"/>
-      <c r="D279" s="10"/>
-      <c r="E279" s="10"/>
-      <c r="F279" s="10"/>
-      <c r="G279" s="10"/>
+      <c r="B279" s="8"/>
+      <c r="C279" s="8"/>
+      <c r="D279" s="8"/>
+      <c r="E279" s="8"/>
+      <c r="F279" s="8"/>
+      <c r="G279" s="8"/>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A280" s="10" t="s">
+      <c r="A280" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B280" s="10"/>
-      <c r="C280" s="10"/>
-      <c r="D280" s="10"/>
-      <c r="E280" s="10"/>
-      <c r="F280" s="10"/>
-      <c r="G280" s="10"/>
+      <c r="B280" s="8"/>
+      <c r="C280" s="8"/>
+      <c r="D280" s="8"/>
+      <c r="E280" s="8"/>
+      <c r="F280" s="8"/>
+      <c r="G280" s="8"/>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281" s="10" t="s">
+      <c r="A281" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B281" s="10"/>
-      <c r="C281" s="10"/>
-      <c r="D281" s="10"/>
-      <c r="E281" s="10"/>
-      <c r="F281" s="10"/>
-      <c r="G281" s="10"/>
+      <c r="B281" s="8"/>
+      <c r="C281" s="8"/>
+      <c r="D281" s="8"/>
+      <c r="E281" s="8"/>
+      <c r="F281" s="8"/>
+      <c r="G281" s="8"/>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="10"/>
-      <c r="B282" s="10"/>
-      <c r="C282" s="10"/>
-      <c r="D282" s="10"/>
-      <c r="E282" s="10"/>
-      <c r="F282" s="10"/>
-      <c r="G282" s="10"/>
+      <c r="A282" s="8"/>
+      <c r="B282" s="8"/>
+      <c r="C282" s="8"/>
+      <c r="D282" s="8"/>
+      <c r="E282" s="8"/>
+      <c r="F282" s="8"/>
+      <c r="G282" s="8"/>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283" s="10"/>
-      <c r="B283" s="10"/>
-      <c r="C283" s="10"/>
-      <c r="D283" s="10"/>
-      <c r="E283" s="10"/>
-      <c r="F283" s="10"/>
-      <c r="G283" s="10"/>
+      <c r="A283" s="8"/>
+      <c r="B283" s="8"/>
+      <c r="C283" s="8"/>
+      <c r="D283" s="8"/>
+      <c r="E283" s="8"/>
+      <c r="F283" s="8"/>
+      <c r="G283" s="8"/>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284" s="8" t="s">
+      <c r="A284" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B284" s="8"/>
-      <c r="C284" s="8"/>
-      <c r="D284" s="10"/>
-      <c r="E284" s="10"/>
-      <c r="F284" s="10"/>
-      <c r="G284" s="10"/>
+      <c r="B284" s="14"/>
+      <c r="C284" s="14"/>
+      <c r="D284" s="8"/>
+      <c r="E284" s="8"/>
+      <c r="F284" s="8"/>
+      <c r="G284" s="8"/>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="10" t="s">
+      <c r="A285" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B285" s="10"/>
-      <c r="C285" s="10"/>
-      <c r="D285" s="10"/>
-      <c r="E285" s="10"/>
-      <c r="F285" s="10"/>
-      <c r="G285" s="10"/>
+      <c r="B285" s="8"/>
+      <c r="C285" s="8"/>
+      <c r="D285" s="8"/>
+      <c r="E285" s="8"/>
+      <c r="F285" s="8"/>
+      <c r="G285" s="8"/>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="10" t="s">
+      <c r="A286" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B286" s="10"/>
-      <c r="C286" s="10"/>
-      <c r="D286" s="10"/>
-      <c r="E286" s="10"/>
-      <c r="F286" s="10"/>
-      <c r="G286" s="10"/>
+      <c r="B286" s="8"/>
+      <c r="C286" s="8"/>
+      <c r="D286" s="8"/>
+      <c r="E286" s="8"/>
+      <c r="F286" s="8"/>
+      <c r="G286" s="8"/>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="10" t="s">
+      <c r="A287" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B287" s="10"/>
-      <c r="C287" s="10"/>
-      <c r="D287" s="10"/>
-      <c r="E287" s="10"/>
-      <c r="F287" s="10"/>
-      <c r="G287" s="10"/>
+      <c r="B287" s="8"/>
+      <c r="C287" s="8"/>
+      <c r="D287" s="8"/>
+      <c r="E287" s="8"/>
+      <c r="F287" s="8"/>
+      <c r="G287" s="8"/>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" s="10" t="s">
+      <c r="A288" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B288" s="10"/>
-      <c r="C288" s="10"/>
-      <c r="D288" s="10"/>
-      <c r="E288" s="10"/>
-      <c r="F288" s="10"/>
-      <c r="G288" s="10"/>
+      <c r="B288" s="8"/>
+      <c r="C288" s="8"/>
+      <c r="D288" s="8"/>
+      <c r="E288" s="8"/>
+      <c r="F288" s="8"/>
+      <c r="G288" s="8"/>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="10" t="s">
+      <c r="A289" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B289" s="10"/>
-      <c r="C289" s="10"/>
-      <c r="D289" s="10"/>
-      <c r="E289" s="10"/>
-      <c r="F289" s="10"/>
-      <c r="G289" s="10"/>
+      <c r="B289" s="8"/>
+      <c r="C289" s="8"/>
+      <c r="D289" s="8"/>
+      <c r="E289" s="8"/>
+      <c r="F289" s="8"/>
+      <c r="G289" s="8"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A290" s="10" t="s">
+      <c r="A290" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B290" s="10"/>
-      <c r="C290" s="10"/>
-      <c r="D290" s="10"/>
-      <c r="E290" s="10"/>
-      <c r="F290" s="10"/>
-      <c r="G290" s="10"/>
+      <c r="B290" s="8"/>
+      <c r="C290" s="8"/>
+      <c r="D290" s="8"/>
+      <c r="E290" s="8"/>
+      <c r="F290" s="8"/>
+      <c r="G290" s="8"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A291" s="10" t="s">
+      <c r="A291" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B291" s="10"/>
-      <c r="C291" s="10"/>
-      <c r="D291" s="10"/>
-      <c r="E291" s="10"/>
-      <c r="F291" s="10"/>
-      <c r="G291" s="10"/>
+      <c r="B291" s="8"/>
+      <c r="C291" s="8"/>
+      <c r="D291" s="8"/>
+      <c r="E291" s="8"/>
+      <c r="F291" s="8"/>
+      <c r="G291" s="8"/>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A292" s="10" t="s">
+      <c r="A292" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B292" s="10"/>
-      <c r="C292" s="10"/>
-      <c r="D292" s="10"/>
-      <c r="E292" s="10"/>
-      <c r="F292" s="10"/>
-      <c r="G292" s="10"/>
+      <c r="B292" s="8"/>
+      <c r="C292" s="8"/>
+      <c r="D292" s="8"/>
+      <c r="E292" s="8"/>
+      <c r="F292" s="8"/>
+      <c r="G292" s="8"/>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A293" s="10" t="s">
+      <c r="A293" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B293" s="10"/>
-      <c r="C293" s="10"/>
-      <c r="D293" s="10"/>
-      <c r="E293" s="10"/>
-      <c r="F293" s="10"/>
-      <c r="G293" s="10"/>
+      <c r="B293" s="8"/>
+      <c r="C293" s="8"/>
+      <c r="D293" s="8"/>
+      <c r="E293" s="8"/>
+      <c r="F293" s="8"/>
+      <c r="G293" s="8"/>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294" s="10" t="s">
+      <c r="A294" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B294" s="10"/>
-      <c r="C294" s="10"/>
-      <c r="D294" s="10"/>
-      <c r="E294" s="10"/>
-      <c r="F294" s="10"/>
-      <c r="G294" s="10"/>
+      <c r="B294" s="8"/>
+      <c r="C294" s="8"/>
+      <c r="D294" s="8"/>
+      <c r="E294" s="8"/>
+      <c r="F294" s="8"/>
+      <c r="G294" s="8"/>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295" s="10" t="s">
+      <c r="A295" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B295" s="10"/>
-      <c r="C295" s="10"/>
-      <c r="D295" s="10"/>
-      <c r="E295" s="10"/>
-      <c r="F295" s="10"/>
-      <c r="G295" s="10"/>
+      <c r="B295" s="8"/>
+      <c r="C295" s="8"/>
+      <c r="D295" s="8"/>
+      <c r="E295" s="8"/>
+      <c r="F295" s="8"/>
+      <c r="G295" s="8"/>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A296" s="10" t="s">
+      <c r="A296" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B296" s="10"/>
-      <c r="C296" s="10"/>
-      <c r="D296" s="10"/>
-      <c r="E296" s="10"/>
-      <c r="F296" s="10"/>
-      <c r="G296" s="10"/>
+      <c r="B296" s="8"/>
+      <c r="C296" s="8"/>
+      <c r="D296" s="8"/>
+      <c r="E296" s="8"/>
+      <c r="F296" s="8"/>
+      <c r="G296" s="8"/>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A297" s="10" t="s">
+      <c r="A297" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B297" s="10"/>
-      <c r="C297" s="10"/>
-      <c r="D297" s="10"/>
-      <c r="E297" s="10"/>
-      <c r="F297" s="10"/>
-      <c r="G297" s="10"/>
+      <c r="B297" s="8"/>
+      <c r="C297" s="8"/>
+      <c r="D297" s="8"/>
+      <c r="E297" s="8"/>
+      <c r="F297" s="8"/>
+      <c r="G297" s="8"/>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A298" s="10" t="s">
+      <c r="A298" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B298" s="10"/>
-      <c r="C298" s="10"/>
-      <c r="D298" s="10"/>
-      <c r="E298" s="10"/>
-      <c r="F298" s="10"/>
-      <c r="G298" s="10"/>
+      <c r="B298" s="8"/>
+      <c r="C298" s="8"/>
+      <c r="D298" s="8"/>
+      <c r="E298" s="8"/>
+      <c r="F298" s="8"/>
+      <c r="G298" s="8"/>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A299" s="10" t="s">
+      <c r="A299" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B299" s="10"/>
-      <c r="C299" s="10"/>
-      <c r="D299" s="10"/>
-      <c r="E299" s="10"/>
-      <c r="F299" s="10"/>
-      <c r="G299" s="10"/>
+      <c r="B299" s="8"/>
+      <c r="C299" s="8"/>
+      <c r="D299" s="8"/>
+      <c r="E299" s="8"/>
+      <c r="F299" s="8"/>
+      <c r="G299" s="8"/>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A300" s="10" t="s">
+      <c r="A300" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B300" s="10"/>
-      <c r="C300" s="10"/>
-      <c r="D300" s="10"/>
-      <c r="E300" s="10"/>
-      <c r="F300" s="10"/>
-      <c r="G300" s="10"/>
+      <c r="B300" s="8"/>
+      <c r="C300" s="8"/>
+      <c r="D300" s="8"/>
+      <c r="E300" s="8"/>
+      <c r="F300" s="8"/>
+      <c r="G300" s="8"/>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A301" s="10" t="s">
+      <c r="A301" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B301" s="10"/>
-      <c r="C301" s="10"/>
-      <c r="D301" s="10"/>
-      <c r="E301" s="10"/>
-      <c r="F301" s="10"/>
-      <c r="G301" s="10"/>
+      <c r="B301" s="8"/>
+      <c r="C301" s="8"/>
+      <c r="D301" s="8"/>
+      <c r="E301" s="8"/>
+      <c r="F301" s="8"/>
+      <c r="G301" s="8"/>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A302" s="10" t="s">
+      <c r="A302" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B302" s="10"/>
-      <c r="C302" s="10"/>
-      <c r="D302" s="10"/>
-      <c r="E302" s="10"/>
-      <c r="F302" s="10"/>
-      <c r="G302" s="10"/>
+      <c r="B302" s="8"/>
+      <c r="C302" s="8"/>
+      <c r="D302" s="8"/>
+      <c r="E302" s="8"/>
+      <c r="F302" s="8"/>
+      <c r="G302" s="8"/>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A303" s="10" t="s">
+      <c r="A303" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B303" s="10"/>
-      <c r="C303" s="10"/>
-      <c r="D303" s="10"/>
-      <c r="E303" s="10"/>
-      <c r="F303" s="10"/>
-      <c r="G303" s="10"/>
+      <c r="B303" s="8"/>
+      <c r="C303" s="8"/>
+      <c r="D303" s="8"/>
+      <c r="E303" s="8"/>
+      <c r="F303" s="8"/>
+      <c r="G303" s="8"/>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A304" s="10"/>
-      <c r="B304" s="10"/>
-      <c r="C304" s="10"/>
-      <c r="D304" s="10"/>
-      <c r="E304" s="10"/>
-      <c r="F304" s="10"/>
-      <c r="G304" s="10"/>
+      <c r="A304" s="8"/>
+      <c r="B304" s="8"/>
+      <c r="C304" s="8"/>
+      <c r="D304" s="8"/>
+      <c r="E304" s="8"/>
+      <c r="F304" s="8"/>
+      <c r="G304" s="8"/>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="11" t="s">
+      <c r="A305" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B305" s="11"/>
-      <c r="C305" s="11"/>
-      <c r="D305" s="10"/>
-      <c r="E305" s="10"/>
-      <c r="F305" s="10"/>
-      <c r="G305" s="10"/>
+      <c r="B305" s="9"/>
+      <c r="C305" s="9"/>
+      <c r="D305" s="8"/>
+      <c r="E305" s="8"/>
+      <c r="F305" s="8"/>
+      <c r="G305" s="8"/>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306" s="10" t="s">
+      <c r="A306" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B306" s="10"/>
-      <c r="C306" s="10"/>
-      <c r="D306" s="10"/>
-      <c r="E306" s="10"/>
-      <c r="F306" s="10"/>
-      <c r="G306" s="10"/>
+      <c r="B306" s="8"/>
+      <c r="C306" s="8"/>
+      <c r="D306" s="8"/>
+      <c r="E306" s="8"/>
+      <c r="F306" s="8"/>
+      <c r="G306" s="8"/>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A307" s="10" t="s">
+      <c r="A307" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="B307" s="10"/>
-      <c r="C307" s="10"/>
-      <c r="D307" s="10"/>
-      <c r="E307" s="10"/>
-      <c r="F307" s="10"/>
-      <c r="G307" s="10"/>
+      <c r="B307" s="8"/>
+      <c r="C307" s="8"/>
+      <c r="D307" s="8"/>
+      <c r="E307" s="8"/>
+      <c r="F307" s="8"/>
+      <c r="G307" s="8"/>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A308" s="10" t="s">
+      <c r="A308" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B308" s="10"/>
-      <c r="C308" s="10"/>
-      <c r="D308" s="10"/>
-      <c r="E308" s="10"/>
-      <c r="F308" s="10"/>
-      <c r="G308" s="10"/>
+      <c r="B308" s="8"/>
+      <c r="C308" s="8"/>
+      <c r="D308" s="8"/>
+      <c r="E308" s="8"/>
+      <c r="F308" s="8"/>
+      <c r="G308" s="8"/>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A309" s="10" t="s">
+      <c r="A309" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B309" s="10"/>
-      <c r="C309" s="10"/>
-      <c r="D309" s="10"/>
-      <c r="E309" s="10"/>
-      <c r="F309" s="10"/>
-      <c r="G309" s="10"/>
+      <c r="B309" s="8"/>
+      <c r="C309" s="8"/>
+      <c r="D309" s="8"/>
+      <c r="E309" s="8"/>
+      <c r="F309" s="8"/>
+      <c r="G309" s="8"/>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A310" s="10" t="s">
+      <c r="A310" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B310" s="10"/>
-      <c r="C310" s="10"/>
-      <c r="D310" s="10"/>
-      <c r="E310" s="10"/>
-      <c r="F310" s="10"/>
-      <c r="G310" s="10"/>
+      <c r="B310" s="8"/>
+      <c r="C310" s="8"/>
+      <c r="D310" s="8"/>
+      <c r="E310" s="8"/>
+      <c r="F310" s="8"/>
+      <c r="G310" s="8"/>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A311" s="10" t="s">
+      <c r="A311" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B311" s="10"/>
-      <c r="C311" s="10"/>
-      <c r="D311" s="10"/>
-      <c r="E311" s="10"/>
-      <c r="F311" s="10"/>
-      <c r="G311" s="10"/>
+      <c r="B311" s="8"/>
+      <c r="C311" s="8"/>
+      <c r="D311" s="8"/>
+      <c r="E311" s="8"/>
+      <c r="F311" s="8"/>
+      <c r="G311" s="8"/>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A312" s="10" t="s">
+      <c r="A312" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B312" s="10"/>
-      <c r="C312" s="10"/>
-      <c r="D312" s="10"/>
-      <c r="E312" s="10"/>
-      <c r="F312" s="10"/>
-      <c r="G312" s="10"/>
+      <c r="B312" s="8"/>
+      <c r="C312" s="8"/>
+      <c r="D312" s="8"/>
+      <c r="E312" s="8"/>
+      <c r="F312" s="8"/>
+      <c r="G312" s="8"/>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A313" s="10" t="s">
+      <c r="A313" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B313" s="10"/>
-      <c r="C313" s="10"/>
-      <c r="D313" s="10"/>
-      <c r="E313" s="10"/>
-      <c r="F313" s="10"/>
-      <c r="G313" s="10"/>
+      <c r="B313" s="8"/>
+      <c r="C313" s="8"/>
+      <c r="D313" s="8"/>
+      <c r="E313" s="8"/>
+      <c r="F313" s="8"/>
+      <c r="G313" s="8"/>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A314" s="10" t="s">
+      <c r="A314" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B314" s="10"/>
-      <c r="C314" s="10"/>
-      <c r="D314" s="10"/>
-      <c r="E314" s="10"/>
-      <c r="F314" s="10"/>
-      <c r="G314" s="10"/>
+      <c r="B314" s="8"/>
+      <c r="C314" s="8"/>
+      <c r="D314" s="8"/>
+      <c r="E314" s="8"/>
+      <c r="F314" s="8"/>
+      <c r="G314" s="8"/>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A315" s="10" t="s">
+      <c r="A315" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B315" s="10"/>
-      <c r="C315" s="10"/>
-      <c r="D315" s="10"/>
-      <c r="E315" s="10"/>
-      <c r="F315" s="10"/>
-      <c r="G315" s="10"/>
+      <c r="B315" s="8"/>
+      <c r="C315" s="8"/>
+      <c r="D315" s="8"/>
+      <c r="E315" s="8"/>
+      <c r="F315" s="8"/>
+      <c r="G315" s="8"/>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A316" s="10" t="s">
+      <c r="A316" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B316" s="10"/>
-      <c r="C316" s="10"/>
-      <c r="D316" s="10"/>
-      <c r="E316" s="10"/>
-      <c r="F316" s="10"/>
-      <c r="G316" s="10"/>
+      <c r="B316" s="8"/>
+      <c r="C316" s="8"/>
+      <c r="D316" s="8"/>
+      <c r="E316" s="8"/>
+      <c r="F316" s="8"/>
+      <c r="G316" s="8"/>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A317" s="10" t="s">
+      <c r="A317" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B317" s="10"/>
-      <c r="C317" s="10"/>
-      <c r="D317" s="10"/>
-      <c r="E317" s="10"/>
-      <c r="F317" s="10"/>
-      <c r="G317" s="10"/>
+      <c r="B317" s="8"/>
+      <c r="C317" s="8"/>
+      <c r="D317" s="8"/>
+      <c r="E317" s="8"/>
+      <c r="F317" s="8"/>
+      <c r="G317" s="8"/>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A318" s="10" t="s">
+      <c r="A318" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B318" s="10"/>
-      <c r="C318" s="10"/>
-      <c r="D318" s="10"/>
-      <c r="E318" s="10"/>
-      <c r="F318" s="10"/>
-      <c r="G318" s="10"/>
+      <c r="B318" s="8"/>
+      <c r="C318" s="8"/>
+      <c r="D318" s="8"/>
+      <c r="E318" s="8"/>
+      <c r="F318" s="8"/>
+      <c r="G318" s="8"/>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A319" s="10" t="s">
+      <c r="A319" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B319" s="10"/>
-      <c r="C319" s="10"/>
-      <c r="D319" s="10"/>
-      <c r="E319" s="10"/>
-      <c r="F319" s="10"/>
-      <c r="G319" s="10"/>
+      <c r="B319" s="8"/>
+      <c r="C319" s="8"/>
+      <c r="D319" s="8"/>
+      <c r="E319" s="8"/>
+      <c r="F319" s="8"/>
+      <c r="G319" s="8"/>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A320" s="10" t="s">
+      <c r="A320" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B320" s="10"/>
-      <c r="C320" s="10"/>
-      <c r="D320" s="10"/>
-      <c r="E320" s="10"/>
-      <c r="F320" s="10"/>
-      <c r="G320" s="10"/>
+      <c r="B320" s="8"/>
+      <c r="C320" s="8"/>
+      <c r="D320" s="8"/>
+      <c r="E320" s="8"/>
+      <c r="F320" s="8"/>
+      <c r="G320" s="8"/>
     </row>
     <row r="321" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A321" s="10" t="s">
+      <c r="A321" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B321" s="10"/>
-      <c r="C321" s="10"/>
-      <c r="D321" s="10"/>
-      <c r="E321" s="10"/>
-      <c r="F321" s="10"/>
-      <c r="G321" s="10"/>
+      <c r="B321" s="8"/>
+      <c r="C321" s="8"/>
+      <c r="D321" s="8"/>
+      <c r="E321" s="8"/>
+      <c r="F321" s="8"/>
+      <c r="G321" s="8"/>
     </row>
     <row r="322" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A322" s="10" t="s">
+      <c r="A322" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B322" s="10"/>
-      <c r="C322" s="10"/>
-      <c r="D322" s="10"/>
-      <c r="E322" s="10"/>
-      <c r="F322" s="10"/>
-      <c r="G322" s="10"/>
+      <c r="B322" s="8"/>
+      <c r="C322" s="8"/>
+      <c r="D322" s="8"/>
+      <c r="E322" s="8"/>
+      <c r="F322" s="8"/>
+      <c r="G322" s="8"/>
     </row>
     <row r="323" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A323" s="10" t="s">
+      <c r="A323" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B323" s="10"/>
-      <c r="C323" s="10"/>
-      <c r="D323" s="10"/>
-      <c r="E323" s="10"/>
-      <c r="F323" s="10"/>
-      <c r="G323" s="10"/>
+      <c r="B323" s="8"/>
+      <c r="C323" s="8"/>
+      <c r="D323" s="8"/>
+      <c r="E323" s="8"/>
+      <c r="F323" s="8"/>
+      <c r="G323" s="8"/>
     </row>
     <row r="324" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A324" s="10" t="s">
+      <c r="A324" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B324" s="10"/>
-      <c r="C324" s="10"/>
-      <c r="D324" s="10"/>
-      <c r="E324" s="10"/>
-      <c r="F324" s="10"/>
-      <c r="G324" s="10"/>
+      <c r="B324" s="8"/>
+      <c r="C324" s="8"/>
+      <c r="D324" s="8"/>
+      <c r="E324" s="8"/>
+      <c r="F324" s="8"/>
+      <c r="G324" s="8"/>
     </row>
     <row r="325" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A325" s="10" t="s">
+      <c r="A325" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B325" s="10"/>
-      <c r="C325" s="10"/>
-      <c r="D325" s="10"/>
-      <c r="E325" s="10"/>
-      <c r="F325" s="10"/>
-      <c r="G325" s="10"/>
+      <c r="B325" s="8"/>
+      <c r="C325" s="8"/>
+      <c r="D325" s="8"/>
+      <c r="E325" s="8"/>
+      <c r="F325" s="8"/>
+      <c r="G325" s="8"/>
     </row>
     <row r="326" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A326" s="10" t="s">
+      <c r="A326" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B326" s="10"/>
-      <c r="C326" s="10"/>
-      <c r="D326" s="10"/>
-      <c r="E326" s="10"/>
-      <c r="F326" s="10"/>
-      <c r="G326" s="10"/>
+      <c r="B326" s="8"/>
+      <c r="C326" s="8"/>
+      <c r="D326" s="8"/>
+      <c r="E326" s="8"/>
+      <c r="F326" s="8"/>
+      <c r="G326" s="8"/>
     </row>
     <row r="327" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A327" s="10" t="s">
+      <c r="A327" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B327" s="10"/>
-      <c r="C327" s="10"/>
-      <c r="D327" s="10"/>
-      <c r="E327" s="10"/>
-      <c r="F327" s="10"/>
-      <c r="G327" s="10"/>
+      <c r="B327" s="8"/>
+      <c r="C327" s="8"/>
+      <c r="D327" s="8"/>
+      <c r="E327" s="8"/>
+      <c r="F327" s="8"/>
+      <c r="G327" s="8"/>
     </row>
     <row r="328" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A328" s="10" t="s">
+      <c r="A328" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B328" s="10"/>
-      <c r="C328" s="10"/>
-      <c r="D328" s="10"/>
-      <c r="E328" s="10"/>
-      <c r="F328" s="10"/>
-      <c r="G328" s="10"/>
+      <c r="B328" s="8"/>
+      <c r="C328" s="8"/>
+      <c r="D328" s="8"/>
+      <c r="E328" s="8"/>
+      <c r="F328" s="8"/>
+      <c r="G328" s="8"/>
     </row>
     <row r="329" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A329" s="10" t="s">
+      <c r="A329" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B329" s="10"/>
-      <c r="C329" s="10"/>
-      <c r="D329" s="10"/>
-      <c r="E329" s="10"/>
-      <c r="F329" s="10"/>
-      <c r="G329" s="10"/>
+      <c r="B329" s="8"/>
+      <c r="C329" s="8"/>
+      <c r="D329" s="8"/>
+      <c r="E329" s="8"/>
+      <c r="F329" s="8"/>
+      <c r="G329" s="8"/>
     </row>
     <row r="330" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A330" s="10" t="s">
+      <c r="A330" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B330" s="10"/>
-      <c r="C330" s="10"/>
-      <c r="D330" s="10"/>
-      <c r="E330" s="10"/>
-      <c r="F330" s="10"/>
-      <c r="G330" s="10"/>
+      <c r="B330" s="8"/>
+      <c r="C330" s="8"/>
+      <c r="D330" s="8"/>
+      <c r="E330" s="8"/>
+      <c r="F330" s="8"/>
+      <c r="G330" s="8"/>
     </row>
     <row r="331" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A331" s="10" t="s">
+      <c r="A331" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B331" s="10"/>
-      <c r="C331" s="10"/>
-      <c r="D331" s="10"/>
-      <c r="E331" s="10"/>
-      <c r="F331" s="10"/>
-      <c r="G331" s="10"/>
+      <c r="B331" s="8"/>
+      <c r="C331" s="8"/>
+      <c r="D331" s="8"/>
+      <c r="E331" s="8"/>
+      <c r="F331" s="8"/>
+      <c r="G331" s="8"/>
     </row>
     <row r="332" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A332" s="10" t="s">
+      <c r="A332" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B332" s="10"/>
-      <c r="C332" s="10"/>
-      <c r="D332" s="10"/>
-      <c r="E332" s="10"/>
-      <c r="F332" s="10"/>
-      <c r="G332" s="10"/>
+      <c r="B332" s="8"/>
+      <c r="C332" s="8"/>
+      <c r="D332" s="8"/>
+      <c r="E332" s="8"/>
+      <c r="F332" s="8"/>
+      <c r="G332" s="8"/>
     </row>
     <row r="333" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A333" s="10" t="s">
+      <c r="A333" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B333" s="10"/>
-      <c r="C333" s="10"/>
-      <c r="D333" s="10"/>
-      <c r="E333" s="10"/>
-      <c r="F333" s="10"/>
-      <c r="G333" s="10"/>
-      <c r="L333" s="13"/>
-      <c r="M333" s="13"/>
-      <c r="N333" s="13"/>
-      <c r="O333" s="13"/>
-      <c r="P333" s="13"/>
+      <c r="B333" s="8"/>
+      <c r="C333" s="8"/>
+      <c r="D333" s="8"/>
+      <c r="E333" s="8"/>
+      <c r="F333" s="8"/>
+      <c r="G333" s="8"/>
+      <c r="L333" s="11"/>
+      <c r="M333" s="11"/>
+      <c r="N333" s="11"/>
+      <c r="O333" s="11"/>
+      <c r="P333" s="11"/>
     </row>
     <row r="334" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A334" s="10" t="s">
+      <c r="A334" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B334" s="10"/>
-      <c r="C334" s="10"/>
-      <c r="D334" s="10"/>
-      <c r="E334" s="10"/>
-      <c r="F334" s="10"/>
-      <c r="G334" s="10"/>
-      <c r="L334" s="13"/>
-      <c r="M334" s="13"/>
-      <c r="N334" s="13"/>
-      <c r="O334" s="13"/>
-      <c r="P334" s="13"/>
+      <c r="B334" s="8"/>
+      <c r="C334" s="8"/>
+      <c r="D334" s="8"/>
+      <c r="E334" s="8"/>
+      <c r="F334" s="8"/>
+      <c r="G334" s="8"/>
+      <c r="L334" s="11"/>
+      <c r="M334" s="11"/>
+      <c r="N334" s="11"/>
+      <c r="O334" s="11"/>
+      <c r="P334" s="11"/>
     </row>
     <row r="335" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A335" s="10" t="s">
+      <c r="A335" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B335" s="10"/>
-      <c r="C335" s="10"/>
-      <c r="D335" s="10"/>
-      <c r="E335" s="10"/>
-      <c r="F335" s="10"/>
-      <c r="G335" s="10"/>
-      <c r="L335" s="13"/>
-      <c r="M335" s="13"/>
-      <c r="N335" s="13"/>
-      <c r="O335" s="13"/>
-      <c r="P335" s="13"/>
+      <c r="B335" s="8"/>
+      <c r="C335" s="8"/>
+      <c r="D335" s="8"/>
+      <c r="E335" s="8"/>
+      <c r="F335" s="8"/>
+      <c r="G335" s="8"/>
+      <c r="L335" s="11"/>
+      <c r="M335" s="11"/>
+      <c r="N335" s="11"/>
+      <c r="O335" s="11"/>
+      <c r="P335" s="11"/>
     </row>
     <row r="336" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A336" s="10" t="s">
+      <c r="A336" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B336" s="10"/>
-      <c r="C336" s="10"/>
-      <c r="D336" s="10"/>
-      <c r="E336" s="10"/>
-      <c r="F336" s="10"/>
-      <c r="G336" s="10"/>
-      <c r="L336" s="13"/>
-      <c r="M336" s="13"/>
-      <c r="N336" s="13"/>
-      <c r="O336" s="13"/>
-      <c r="P336" s="13"/>
+      <c r="B336" s="8"/>
+      <c r="C336" s="8"/>
+      <c r="D336" s="8"/>
+      <c r="E336" s="8"/>
+      <c r="F336" s="8"/>
+      <c r="G336" s="8"/>
+      <c r="L336" s="11"/>
+      <c r="M336" s="11"/>
+      <c r="N336" s="11"/>
+      <c r="O336" s="11"/>
+      <c r="P336" s="11"/>
     </row>
     <row r="337" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A337" s="10" t="s">
+      <c r="A337" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B337" s="10"/>
-      <c r="C337" s="10"/>
-      <c r="D337" s="10"/>
-      <c r="E337" s="10"/>
-      <c r="F337" s="10"/>
-      <c r="G337" s="10"/>
-      <c r="L337" s="13"/>
-      <c r="M337" s="13"/>
-      <c r="N337" s="13"/>
-      <c r="O337" s="13"/>
-      <c r="P337" s="13"/>
+      <c r="B337" s="8"/>
+      <c r="C337" s="8"/>
+      <c r="D337" s="8"/>
+      <c r="E337" s="8"/>
+      <c r="F337" s="8"/>
+      <c r="G337" s="8"/>
+      <c r="L337" s="11"/>
+      <c r="M337" s="11"/>
+      <c r="N337" s="11"/>
+      <c r="O337" s="11"/>
+      <c r="P337" s="11"/>
     </row>
     <row r="338" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A338" s="10" t="s">
+      <c r="A338" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B338" s="10"/>
-      <c r="C338" s="10"/>
-      <c r="D338" s="10"/>
-      <c r="E338" s="10"/>
-      <c r="F338" s="10"/>
-      <c r="G338" s="10"/>
-      <c r="L338" s="13"/>
-      <c r="M338" s="13"/>
-      <c r="N338" s="14"/>
-      <c r="O338" s="13"/>
-      <c r="P338" s="13"/>
+      <c r="B338" s="8"/>
+      <c r="C338" s="8"/>
+      <c r="D338" s="8"/>
+      <c r="E338" s="8"/>
+      <c r="F338" s="8"/>
+      <c r="G338" s="8"/>
+      <c r="L338" s="11"/>
+      <c r="M338" s="11"/>
+      <c r="N338" s="12"/>
+      <c r="O338" s="11"/>
+      <c r="P338" s="11"/>
     </row>
     <row r="339" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A339" s="11" t="s">
+      <c r="A339" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B339" s="10"/>
-      <c r="C339" s="10"/>
-      <c r="D339" s="10"/>
-      <c r="E339" s="10"/>
-      <c r="F339" s="10"/>
-      <c r="G339" s="10"/>
-      <c r="L339" s="13"/>
-      <c r="M339" s="13"/>
-      <c r="N339" s="13"/>
-      <c r="O339" s="13"/>
-      <c r="P339" s="13"/>
+      <c r="B339" s="8"/>
+      <c r="C339" s="8"/>
+      <c r="D339" s="8"/>
+      <c r="E339" s="8"/>
+      <c r="F339" s="8"/>
+      <c r="G339" s="8"/>
+      <c r="L339" s="11"/>
+      <c r="M339" s="11"/>
+      <c r="N339" s="11"/>
+      <c r="O339" s="11"/>
+      <c r="P339" s="11"/>
     </row>
     <row r="340" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A340" s="10" t="s">
+      <c r="A340" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B340" s="10"/>
-      <c r="C340" s="10"/>
-      <c r="D340" s="10"/>
-      <c r="E340" s="10"/>
-      <c r="F340" s="10"/>
-      <c r="G340" s="10"/>
-      <c r="L340" s="13"/>
-      <c r="M340" s="13"/>
-      <c r="N340" s="13"/>
-      <c r="O340" s="13"/>
-      <c r="P340" s="13"/>
+      <c r="B340" s="8"/>
+      <c r="C340" s="8"/>
+      <c r="D340" s="8"/>
+      <c r="E340" s="8"/>
+      <c r="F340" s="8"/>
+      <c r="G340" s="8"/>
+      <c r="L340" s="11"/>
+      <c r="M340" s="11"/>
+      <c r="N340" s="11"/>
+      <c r="O340" s="11"/>
+      <c r="P340" s="11"/>
     </row>
     <row r="341" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A341" s="10"/>
-      <c r="B341" s="10"/>
-      <c r="C341" s="10"/>
-      <c r="D341" s="10"/>
-      <c r="E341" s="10"/>
-      <c r="F341" s="10"/>
-      <c r="G341" s="10"/>
-      <c r="L341" s="13"/>
-      <c r="M341" s="13"/>
-      <c r="N341" s="13"/>
-      <c r="O341" s="13"/>
-      <c r="P341" s="13"/>
+      <c r="A341" s="8"/>
+      <c r="B341" s="8"/>
+      <c r="C341" s="8"/>
+      <c r="D341" s="8"/>
+      <c r="E341" s="8"/>
+      <c r="F341" s="8"/>
+      <c r="G341" s="8"/>
+      <c r="L341" s="11"/>
+      <c r="M341" s="11"/>
+      <c r="N341" s="11"/>
+      <c r="O341" s="11"/>
+      <c r="P341" s="11"/>
     </row>
     <row r="342" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A342" s="12" t="s">
+      <c r="A342" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B342" s="10"/>
-      <c r="C342" s="10"/>
-      <c r="D342" s="10"/>
-      <c r="E342" s="10"/>
-      <c r="F342" s="10"/>
-      <c r="G342" s="10"/>
-      <c r="L342" s="13"/>
-      <c r="M342" s="13"/>
-      <c r="N342" s="13"/>
-      <c r="O342" s="13"/>
-      <c r="P342" s="13"/>
+      <c r="B342" s="8"/>
+      <c r="C342" s="8"/>
+      <c r="D342" s="8"/>
+      <c r="E342" s="8"/>
+      <c r="F342" s="8"/>
+      <c r="G342" s="8"/>
+      <c r="L342" s="11"/>
+      <c r="M342" s="11"/>
+      <c r="N342" s="11"/>
+      <c r="O342" s="11"/>
+      <c r="P342" s="11"/>
     </row>
     <row r="343" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A343" s="10" t="s">
+      <c r="A343" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B343" s="10"/>
-      <c r="C343" s="10"/>
-      <c r="D343" s="10"/>
-      <c r="E343" s="10"/>
-      <c r="F343" s="10"/>
-      <c r="G343" s="10"/>
-      <c r="L343" s="13"/>
-      <c r="M343" s="13"/>
-      <c r="N343" s="13"/>
-      <c r="O343" s="13"/>
-      <c r="P343" s="13"/>
+      <c r="B343" s="8"/>
+      <c r="C343" s="8"/>
+      <c r="D343" s="8"/>
+      <c r="E343" s="8"/>
+      <c r="F343" s="8"/>
+      <c r="G343" s="8"/>
+      <c r="L343" s="11"/>
+      <c r="M343" s="11"/>
+      <c r="N343" s="11"/>
+      <c r="O343" s="11"/>
+      <c r="P343" s="11"/>
     </row>
     <row r="344" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A344" s="10" t="s">
+      <c r="A344" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B344" s="10"/>
-      <c r="C344" s="10"/>
-      <c r="D344" s="10"/>
-      <c r="E344" s="10"/>
-      <c r="F344" s="10"/>
-      <c r="G344" s="10"/>
-      <c r="L344" s="13"/>
-      <c r="M344" s="13"/>
-      <c r="N344" s="13"/>
-      <c r="O344" s="13"/>
-      <c r="P344" s="13"/>
+      <c r="B344" s="8"/>
+      <c r="C344" s="8"/>
+      <c r="D344" s="8"/>
+      <c r="E344" s="8"/>
+      <c r="F344" s="8"/>
+      <c r="G344" s="8"/>
+      <c r="L344" s="11"/>
+      <c r="M344" s="11"/>
+      <c r="N344" s="11"/>
+      <c r="O344" s="11"/>
+      <c r="P344" s="11"/>
     </row>
     <row r="345" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A345" s="10" t="s">
+      <c r="A345" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B345" s="10"/>
-      <c r="C345" s="10"/>
-      <c r="D345" s="10"/>
-      <c r="E345" s="10"/>
-      <c r="F345" s="10"/>
-      <c r="G345" s="10"/>
-      <c r="L345" s="13"/>
-      <c r="M345" s="13"/>
-      <c r="N345" s="13"/>
-      <c r="O345" s="13"/>
-      <c r="P345" s="13"/>
+      <c r="B345" s="8"/>
+      <c r="C345" s="8"/>
+      <c r="D345" s="8"/>
+      <c r="E345" s="8"/>
+      <c r="F345" s="8"/>
+      <c r="G345" s="8"/>
+      <c r="L345" s="11"/>
+      <c r="M345" s="11"/>
+      <c r="N345" s="11"/>
+      <c r="O345" s="11"/>
+      <c r="P345" s="11"/>
     </row>
     <row r="346" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A346" s="10"/>
-      <c r="B346" s="10"/>
-      <c r="C346" s="10"/>
-      <c r="D346" s="10"/>
-      <c r="E346" s="10"/>
-      <c r="F346" s="10"/>
-      <c r="G346" s="10"/>
-      <c r="L346" s="13"/>
-      <c r="M346" s="13"/>
-      <c r="N346" s="13"/>
-      <c r="O346" s="13"/>
-      <c r="P346" s="13"/>
+      <c r="A346" s="8"/>
+      <c r="B346" s="8"/>
+      <c r="C346" s="8"/>
+      <c r="D346" s="8"/>
+      <c r="E346" s="8"/>
+      <c r="F346" s="8"/>
+      <c r="G346" s="8"/>
+      <c r="L346" s="11"/>
+      <c r="M346" s="11"/>
+      <c r="N346" s="11"/>
+      <c r="O346" s="11"/>
+      <c r="P346" s="11"/>
     </row>
     <row r="347" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A347" s="10"/>
-      <c r="B347" s="10"/>
-      <c r="C347" s="10"/>
-      <c r="D347" s="10"/>
-      <c r="E347" s="10"/>
-      <c r="F347" s="10"/>
-      <c r="G347" s="10"/>
-      <c r="L347" s="13"/>
-      <c r="M347" s="13"/>
-      <c r="N347" s="13"/>
-      <c r="O347" s="13"/>
-      <c r="P347" s="13"/>
+      <c r="A347" s="8"/>
+      <c r="B347" s="8"/>
+      <c r="C347" s="8"/>
+      <c r="D347" s="8"/>
+      <c r="E347" s="8"/>
+      <c r="F347" s="8"/>
+      <c r="G347" s="8"/>
+      <c r="L347" s="11"/>
+      <c r="M347" s="11"/>
+      <c r="N347" s="11"/>
+      <c r="O347" s="11"/>
+      <c r="P347" s="11"/>
     </row>
     <row r="348" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A348" s="11" t="s">
+      <c r="A348" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B348" s="10"/>
-      <c r="C348" s="10"/>
-      <c r="D348" s="10"/>
-      <c r="E348" s="10"/>
-      <c r="F348" s="10"/>
-      <c r="G348" s="10"/>
+      <c r="B348" s="8"/>
+      <c r="C348" s="8"/>
+      <c r="D348" s="8"/>
+      <c r="E348" s="8"/>
+      <c r="F348" s="8"/>
+      <c r="G348" s="8"/>
     </row>
     <row r="349" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A349" s="10" t="s">
+      <c r="A349" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B349" s="10"/>
-      <c r="C349" s="10"/>
-      <c r="D349" s="10"/>
-      <c r="E349" s="10"/>
-      <c r="F349" s="10"/>
-      <c r="G349" s="10"/>
+      <c r="B349" s="8"/>
+      <c r="C349" s="8"/>
+      <c r="D349" s="8"/>
+      <c r="E349" s="8"/>
+      <c r="F349" s="8"/>
+      <c r="G349" s="8"/>
     </row>
     <row r="350" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A350" s="10" t="s">
+      <c r="A350" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B350" s="10"/>
-      <c r="C350" s="10"/>
-      <c r="D350" s="10"/>
-      <c r="E350" s="10"/>
-      <c r="F350" s="10"/>
-      <c r="G350" s="10"/>
+      <c r="B350" s="8"/>
+      <c r="C350" s="8"/>
+      <c r="D350" s="8"/>
+      <c r="E350" s="8"/>
+      <c r="F350" s="8"/>
+      <c r="G350" s="8"/>
     </row>
     <row r="351" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A351" s="10" t="s">
+      <c r="A351" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B351" s="10"/>
-      <c r="C351" s="10"/>
-      <c r="D351" s="10"/>
-      <c r="E351" s="10"/>
-      <c r="F351" s="10"/>
-      <c r="G351" s="10"/>
+      <c r="B351" s="8"/>
+      <c r="C351" s="8"/>
+      <c r="D351" s="8"/>
+      <c r="E351" s="8"/>
+      <c r="F351" s="8"/>
+      <c r="G351" s="8"/>
     </row>
     <row r="352" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A352" s="10" t="s">
+      <c r="A352" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B352" s="10"/>
-      <c r="C352" s="10"/>
-      <c r="D352" s="10"/>
-      <c r="E352" s="10"/>
-      <c r="F352" s="10"/>
-      <c r="G352" s="10"/>
+      <c r="B352" s="8"/>
+      <c r="C352" s="8"/>
+      <c r="D352" s="8"/>
+      <c r="E352" s="8"/>
+      <c r="F352" s="8"/>
+      <c r="G352" s="8"/>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A353" s="10" t="s">
+      <c r="A353" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B353" s="10"/>
-      <c r="C353" s="10"/>
-      <c r="D353" s="10"/>
-      <c r="E353" s="10"/>
-      <c r="F353" s="10"/>
-      <c r="G353" s="10"/>
+      <c r="B353" s="8"/>
+      <c r="C353" s="8"/>
+      <c r="D353" s="8"/>
+      <c r="E353" s="8"/>
+      <c r="F353" s="8"/>
+      <c r="G353" s="8"/>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A354" s="10" t="s">
+      <c r="A354" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B354" s="10"/>
-      <c r="C354" s="10"/>
-      <c r="D354" s="10"/>
-      <c r="E354" s="10"/>
-      <c r="F354" s="10"/>
-      <c r="G354" s="10"/>
+      <c r="B354" s="8"/>
+      <c r="C354" s="8"/>
+      <c r="D354" s="8"/>
+      <c r="E354" s="8"/>
+      <c r="F354" s="8"/>
+      <c r="G354" s="8"/>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A355" s="10" t="s">
+      <c r="A355" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B355" s="10"/>
-      <c r="C355" s="10"/>
-      <c r="D355" s="10"/>
-      <c r="E355" s="10"/>
-      <c r="F355" s="10"/>
-      <c r="G355" s="10"/>
+      <c r="B355" s="8"/>
+      <c r="C355" s="8"/>
+      <c r="D355" s="8"/>
+      <c r="E355" s="8"/>
+      <c r="F355" s="8"/>
+      <c r="G355" s="8"/>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A356" s="10" t="s">
+      <c r="A356" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B356" s="10"/>
-      <c r="C356" s="10"/>
-      <c r="D356" s="10"/>
-      <c r="E356" s="10"/>
-      <c r="F356" s="10"/>
-      <c r="G356" s="10"/>
+      <c r="B356" s="8"/>
+      <c r="C356" s="8"/>
+      <c r="D356" s="8"/>
+      <c r="E356" s="8"/>
+      <c r="F356" s="8"/>
+      <c r="G356" s="8"/>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A357" s="10" t="s">
+      <c r="A357" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B357" s="10"/>
-      <c r="C357" s="10"/>
-      <c r="D357" s="10"/>
-      <c r="E357" s="10"/>
-      <c r="F357" s="10"/>
-      <c r="G357" s="10"/>
+      <c r="B357" s="8"/>
+      <c r="C357" s="8"/>
+      <c r="D357" s="8"/>
+      <c r="E357" s="8"/>
+      <c r="F357" s="8"/>
+      <c r="G357" s="8"/>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A358" s="10" t="s">
+      <c r="A358" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B358" s="10"/>
-      <c r="C358" s="10"/>
-      <c r="D358" s="10"/>
-      <c r="E358" s="10"/>
-      <c r="F358" s="10"/>
-      <c r="G358" s="10"/>
+      <c r="B358" s="8"/>
+      <c r="C358" s="8"/>
+      <c r="D358" s="8"/>
+      <c r="E358" s="8"/>
+      <c r="F358" s="8"/>
+      <c r="G358" s="8"/>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A359" s="10"/>
-      <c r="B359" s="10"/>
-      <c r="C359" s="10"/>
-      <c r="D359" s="10"/>
-      <c r="E359" s="10"/>
-      <c r="F359" s="10"/>
-      <c r="G359" s="10"/>
+      <c r="A359" s="8"/>
+      <c r="B359" s="8"/>
+      <c r="C359" s="8"/>
+      <c r="D359" s="8"/>
+      <c r="E359" s="8"/>
+      <c r="F359" s="8"/>
+      <c r="G359" s="8"/>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A360" s="10"/>
-      <c r="B360" s="10"/>
-      <c r="C360" s="10"/>
-      <c r="D360" s="10"/>
-      <c r="E360" s="10"/>
-      <c r="F360" s="10"/>
-      <c r="G360" s="10"/>
+      <c r="A360" s="8"/>
+      <c r="B360" s="8"/>
+      <c r="C360" s="8"/>
+      <c r="D360" s="8"/>
+      <c r="E360" s="8"/>
+      <c r="F360" s="8"/>
+      <c r="G360" s="8"/>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A361" s="11" t="s">
+      <c r="A361" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B361" s="10"/>
-      <c r="C361" s="10"/>
-      <c r="D361" s="10"/>
-      <c r="E361" s="10"/>
-      <c r="F361" s="10"/>
-      <c r="G361" s="10"/>
+      <c r="B361" s="8"/>
+      <c r="C361" s="8"/>
+      <c r="D361" s="8"/>
+      <c r="E361" s="8"/>
+      <c r="F361" s="8"/>
+      <c r="G361" s="8"/>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A362" s="10" t="s">
+      <c r="A362" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B362" s="10"/>
-      <c r="C362" s="10"/>
-      <c r="D362" s="10"/>
-      <c r="E362" s="10"/>
-      <c r="F362" s="10"/>
-      <c r="G362" s="10"/>
+      <c r="B362" s="8"/>
+      <c r="C362" s="8"/>
+      <c r="D362" s="8"/>
+      <c r="E362" s="8"/>
+      <c r="F362" s="8"/>
+      <c r="G362" s="8"/>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A363" s="10" t="s">
+      <c r="A363" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B363" s="10"/>
-      <c r="C363" s="10"/>
-      <c r="D363" s="10"/>
-      <c r="E363" s="10"/>
-      <c r="F363" s="10"/>
-      <c r="G363" s="10"/>
+      <c r="B363" s="8"/>
+      <c r="C363" s="8"/>
+      <c r="D363" s="8"/>
+      <c r="E363" s="8"/>
+      <c r="F363" s="8"/>
+      <c r="G363" s="8"/>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A364" s="10" t="s">
+      <c r="A364" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B364" s="10"/>
-      <c r="C364" s="10"/>
-      <c r="D364" s="10"/>
-      <c r="E364" s="10"/>
-      <c r="F364" s="10"/>
-      <c r="G364" s="10"/>
+      <c r="B364" s="8"/>
+      <c r="C364" s="8"/>
+      <c r="D364" s="8"/>
+      <c r="E364" s="8"/>
+      <c r="F364" s="8"/>
+      <c r="G364" s="8"/>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A365" s="10" t="s">
+      <c r="A365" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B365" s="10"/>
-      <c r="C365" s="10"/>
-      <c r="D365" s="10"/>
-      <c r="E365" s="10"/>
-      <c r="F365" s="10"/>
-      <c r="G365" s="10"/>
+      <c r="B365" s="8"/>
+      <c r="C365" s="8"/>
+      <c r="D365" s="8"/>
+      <c r="E365" s="8"/>
+      <c r="F365" s="8"/>
+      <c r="G365" s="8"/>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A366" s="10" t="s">
+      <c r="A366" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B366" s="10"/>
-      <c r="C366" s="10"/>
-      <c r="D366" s="10"/>
-      <c r="E366" s="10"/>
-      <c r="F366" s="10"/>
-      <c r="G366" s="10"/>
+      <c r="B366" s="8"/>
+      <c r="C366" s="8"/>
+      <c r="D366" s="8"/>
+      <c r="E366" s="8"/>
+      <c r="F366" s="8"/>
+      <c r="G366" s="8"/>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A367" s="10" t="s">
+      <c r="A367" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B367" s="10"/>
-      <c r="C367" s="10"/>
-      <c r="D367" s="10"/>
-      <c r="E367" s="10"/>
-      <c r="F367" s="10"/>
-      <c r="G367" s="10"/>
+      <c r="B367" s="8"/>
+      <c r="C367" s="8"/>
+      <c r="D367" s="8"/>
+      <c r="E367" s="8"/>
+      <c r="F367" s="8"/>
+      <c r="G367" s="8"/>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A368" s="10" t="s">
+      <c r="A368" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B368" s="10"/>
-      <c r="C368" s="10"/>
-      <c r="D368" s="10"/>
-      <c r="E368" s="10"/>
-      <c r="F368" s="10"/>
-      <c r="G368" s="10"/>
+      <c r="B368" s="8"/>
+      <c r="C368" s="8"/>
+      <c r="D368" s="8"/>
+      <c r="E368" s="8"/>
+      <c r="F368" s="8"/>
+      <c r="G368" s="8"/>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A369" s="10" t="s">
+      <c r="A369" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B369" s="10"/>
-      <c r="C369" s="10"/>
-      <c r="D369" s="10"/>
-      <c r="E369" s="10"/>
-      <c r="F369" s="10"/>
-      <c r="G369" s="10"/>
+      <c r="B369" s="8"/>
+      <c r="C369" s="8"/>
+      <c r="D369" s="8"/>
+      <c r="E369" s="8"/>
+      <c r="F369" s="8"/>
+      <c r="G369" s="8"/>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A370" s="10" t="s">
+      <c r="A370" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B370" s="10"/>
-      <c r="C370" s="10"/>
-      <c r="D370" s="10"/>
-      <c r="E370" s="10"/>
-      <c r="F370" s="10"/>
-      <c r="G370" s="10"/>
+      <c r="B370" s="8"/>
+      <c r="C370" s="8"/>
+      <c r="D370" s="8"/>
+      <c r="E370" s="8"/>
+      <c r="F370" s="8"/>
+      <c r="G370" s="8"/>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A371" s="10" t="s">
+      <c r="A371" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B371" s="10"/>
-      <c r="C371" s="10"/>
-      <c r="D371" s="10"/>
-      <c r="E371" s="10"/>
-      <c r="F371" s="10"/>
-      <c r="G371" s="10"/>
+      <c r="B371" s="8"/>
+      <c r="C371" s="8"/>
+      <c r="D371" s="8"/>
+      <c r="E371" s="8"/>
+      <c r="F371" s="8"/>
+      <c r="G371" s="8"/>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A372" s="10" t="s">
+      <c r="A372" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B372" s="10"/>
-      <c r="C372" s="10"/>
-      <c r="D372" s="10"/>
-      <c r="E372" s="10"/>
-      <c r="F372" s="10"/>
-      <c r="G372" s="10"/>
+      <c r="B372" s="8"/>
+      <c r="C372" s="8"/>
+      <c r="D372" s="8"/>
+      <c r="E372" s="8"/>
+      <c r="F372" s="8"/>
+      <c r="G372" s="8"/>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A373" s="10" t="s">
+      <c r="A373" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B373" s="10"/>
-      <c r="C373" s="10"/>
-      <c r="D373" s="10"/>
-      <c r="E373" s="10"/>
-      <c r="F373" s="10"/>
-      <c r="G373" s="10"/>
+      <c r="B373" s="8"/>
+      <c r="C373" s="8"/>
+      <c r="D373" s="8"/>
+      <c r="E373" s="8"/>
+      <c r="F373" s="8"/>
+      <c r="G373" s="8"/>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A374" s="10" t="s">
+      <c r="A374" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B374" s="10"/>
-      <c r="C374" s="10"/>
-      <c r="D374" s="10"/>
-      <c r="E374" s="10"/>
-      <c r="F374" s="10"/>
-      <c r="G374" s="10"/>
+      <c r="B374" s="8"/>
+      <c r="C374" s="8"/>
+      <c r="D374" s="8"/>
+      <c r="E374" s="8"/>
+      <c r="F374" s="8"/>
+      <c r="G374" s="8"/>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A375" s="10" t="s">
+      <c r="A375" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B375" s="10"/>
-      <c r="C375" s="10"/>
-      <c r="D375" s="10"/>
-      <c r="E375" s="10"/>
-      <c r="F375" s="10"/>
-      <c r="G375" s="10"/>
+      <c r="B375" s="8"/>
+      <c r="C375" s="8"/>
+      <c r="D375" s="8"/>
+      <c r="E375" s="8"/>
+      <c r="F375" s="8"/>
+      <c r="G375" s="8"/>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A376" s="10" t="s">
+      <c r="A376" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B376" s="10"/>
-      <c r="C376" s="10"/>
-      <c r="D376" s="10"/>
-      <c r="E376" s="10"/>
-      <c r="F376" s="10"/>
-      <c r="G376" s="10"/>
+      <c r="B376" s="8"/>
+      <c r="C376" s="8"/>
+      <c r="D376" s="8"/>
+      <c r="E376" s="8"/>
+      <c r="F376" s="8"/>
+      <c r="G376" s="8"/>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A377" s="10" t="s">
+      <c r="A377" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B377" s="10"/>
-      <c r="C377" s="10"/>
-      <c r="D377" s="10"/>
-      <c r="E377" s="10"/>
-      <c r="F377" s="10"/>
-      <c r="G377" s="10"/>
+      <c r="B377" s="8"/>
+      <c r="C377" s="8"/>
+      <c r="D377" s="8"/>
+      <c r="E377" s="8"/>
+      <c r="F377" s="8"/>
+      <c r="G377" s="8"/>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A378" s="10" t="s">
+      <c r="A378" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B378" s="10"/>
-      <c r="C378" s="10"/>
-      <c r="D378" s="10"/>
-      <c r="E378" s="10"/>
-      <c r="F378" s="10"/>
-      <c r="G378" s="10"/>
+      <c r="B378" s="8"/>
+      <c r="C378" s="8"/>
+      <c r="D378" s="8"/>
+      <c r="E378" s="8"/>
+      <c r="F378" s="8"/>
+      <c r="G378" s="8"/>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A379" s="10" t="s">
+      <c r="A379" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B379" s="10"/>
-      <c r="C379" s="10"/>
-      <c r="D379" s="10"/>
-      <c r="E379" s="10"/>
-      <c r="F379" s="10"/>
-      <c r="G379" s="10"/>
+      <c r="B379" s="8"/>
+      <c r="C379" s="8"/>
+      <c r="D379" s="8"/>
+      <c r="E379" s="8"/>
+      <c r="F379" s="8"/>
+      <c r="G379" s="8"/>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A383" s="6" t="s">
+      <c r="A383" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B383" s="6"/>
-      <c r="C383" s="6"/>
-      <c r="D383" s="6"/>
-      <c r="E383" s="6"/>
-      <c r="F383" s="6"/>
-      <c r="G383" s="6"/>
+      <c r="B383" s="13"/>
+      <c r="C383" s="13"/>
+      <c r="D383" s="13"/>
+      <c r="E383" s="13"/>
+      <c r="F383" s="13"/>
+      <c r="G383" s="13"/>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A384" s="7" t="s">
+      <c r="A384" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B384" s="3"/>
@@ -5019,7 +5078,7 @@
       <c r="G389" s="3"/>
     </row>
     <row r="390" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A390" s="7" t="s">
+      <c r="A390" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B390" s="3"/>
@@ -5116,7 +5175,7 @@
       <c r="G398" s="3"/>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A399" s="7" t="s">
+      <c r="A399" s="6" t="s">
         <v>164</v>
       </c>
       <c r="B399" s="3"/>
@@ -5191,7 +5250,7 @@
       <c r="G405" s="3"/>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A406" s="7" t="s">
+      <c r="A406" s="6" t="s">
         <v>96</v>
       </c>
       <c r="B406" s="3"/>
@@ -5321,7 +5380,7 @@
       <c r="G417" s="3"/>
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A418" s="7" t="s">
+      <c r="A418" s="6" t="s">
         <v>175</v>
       </c>
       <c r="B418" s="3"/>
@@ -5529,19 +5588,893 @@
       <c r="F436" s="3"/>
       <c r="G436" s="3"/>
     </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A440" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B440" s="13"/>
+      <c r="C440" s="13"/>
+      <c r="D440" s="13"/>
+      <c r="E440" s="13"/>
+      <c r="F440" s="13"/>
+      <c r="G440" s="13"/>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A441" s="17"/>
+      <c r="B441" s="17"/>
+      <c r="C441" s="17"/>
+      <c r="D441" s="17"/>
+      <c r="E441" s="17"/>
+      <c r="F441" s="17"/>
+      <c r="G441" s="17"/>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A442" s="1"/>
+      <c r="B442" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C442" s="17"/>
+      <c r="D442" s="17"/>
+      <c r="E442" s="17"/>
+      <c r="F442" s="17"/>
+      <c r="G442" s="17"/>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A443" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B443" s="1"/>
+      <c r="C443" s="1"/>
+      <c r="D443" s="1"/>
+      <c r="E443" s="1"/>
+      <c r="F443" s="1"/>
+      <c r="G443" s="1"/>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B444" s="1"/>
+      <c r="C444" s="1"/>
+      <c r="D444" s="1"/>
+      <c r="E444" s="1"/>
+      <c r="F444" s="1"/>
+      <c r="G444" s="1"/>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A445" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B445" s="1"/>
+      <c r="C445" s="1"/>
+      <c r="D445" s="1"/>
+      <c r="E445" s="1"/>
+      <c r="F445" s="1"/>
+      <c r="G445" s="1"/>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B446" s="1"/>
+      <c r="C446" s="1"/>
+      <c r="D446" s="1"/>
+      <c r="E446" s="1"/>
+      <c r="F446" s="1"/>
+      <c r="G446" s="1"/>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A447" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B447" s="1"/>
+      <c r="C447" s="1"/>
+      <c r="D447" s="1"/>
+      <c r="E447" s="1"/>
+      <c r="F447" s="1"/>
+      <c r="G447" s="1"/>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A448" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B448" s="1"/>
+      <c r="C448" s="1"/>
+      <c r="D448" s="1"/>
+      <c r="E448" s="1"/>
+      <c r="F448" s="1"/>
+      <c r="G448" s="1"/>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A449" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B449" s="1"/>
+      <c r="C449" s="1"/>
+      <c r="D449" s="1"/>
+      <c r="E449" s="1"/>
+      <c r="F449" s="1"/>
+      <c r="G449" s="1"/>
+    </row>
+    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A450" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B450" s="1"/>
+      <c r="C450" s="1"/>
+      <c r="D450" s="1"/>
+      <c r="E450" s="1"/>
+      <c r="F450" s="1"/>
+      <c r="G450" s="1"/>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A451" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B451" s="1"/>
+      <c r="C451" s="1"/>
+      <c r="D451" s="1"/>
+      <c r="E451" s="1"/>
+      <c r="F451" s="1"/>
+      <c r="G451" s="1"/>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A452" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B452" s="1"/>
+      <c r="C452" s="1"/>
+      <c r="D452" s="1"/>
+      <c r="E452" s="1"/>
+      <c r="F452" s="1"/>
+      <c r="G452" s="1"/>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A453" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B453" s="1"/>
+      <c r="C453" s="1"/>
+      <c r="D453" s="1"/>
+      <c r="E453" s="1"/>
+      <c r="F453" s="1"/>
+      <c r="G453" s="1"/>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B454" s="1"/>
+      <c r="C454" s="1"/>
+      <c r="D454" s="1"/>
+      <c r="E454" s="1"/>
+      <c r="F454" s="1"/>
+      <c r="G454" s="1"/>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B455" s="1"/>
+      <c r="C455" s="1"/>
+      <c r="D455" s="1"/>
+      <c r="E455" s="1"/>
+      <c r="F455" s="1"/>
+      <c r="G455" s="1"/>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A456" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B456" s="1"/>
+      <c r="C456" s="1"/>
+      <c r="D456" s="1"/>
+      <c r="E456" s="1"/>
+      <c r="F456" s="1"/>
+      <c r="G456" s="1"/>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A457" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B457" s="1"/>
+      <c r="C457" s="1"/>
+      <c r="D457" s="1"/>
+      <c r="E457" s="1"/>
+      <c r="F457" s="1"/>
+      <c r="G457" s="1"/>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A458" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B458" s="1"/>
+      <c r="C458" s="1"/>
+      <c r="D458" s="1"/>
+      <c r="E458" s="1"/>
+      <c r="F458" s="1"/>
+      <c r="G458" s="1"/>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A459" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B459" s="1"/>
+      <c r="C459" s="1"/>
+      <c r="D459" s="1"/>
+      <c r="E459" s="1"/>
+      <c r="F459" s="1"/>
+      <c r="G459" s="1"/>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A460" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B460" s="1"/>
+      <c r="C460" s="1"/>
+      <c r="D460" s="1"/>
+      <c r="E460" s="1"/>
+      <c r="F460" s="1"/>
+      <c r="G460" s="1"/>
+    </row>
+    <row r="461" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A461" s="1"/>
+      <c r="B461" s="1"/>
+      <c r="C461" s="1"/>
+      <c r="D461" s="1"/>
+      <c r="E461" s="1"/>
+      <c r="F461" s="1"/>
+      <c r="G461" s="1"/>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A462" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B462" s="1"/>
+      <c r="C462" s="1"/>
+      <c r="D462" s="1"/>
+      <c r="E462" s="1"/>
+      <c r="F462" s="1"/>
+      <c r="G462" s="1"/>
+    </row>
+    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A463" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B463" s="1"/>
+      <c r="C463" s="1"/>
+      <c r="D463" s="1"/>
+      <c r="E463" s="1"/>
+      <c r="F463" s="1"/>
+      <c r="G463" s="1"/>
+    </row>
+    <row r="464" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A464" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B464" s="1"/>
+      <c r="C464" s="1"/>
+      <c r="D464" s="1"/>
+      <c r="E464" s="1"/>
+      <c r="F464" s="1"/>
+      <c r="G464" s="1"/>
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A465" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B465" s="1"/>
+      <c r="C465" s="1"/>
+      <c r="D465" s="1"/>
+      <c r="E465" s="1"/>
+      <c r="F465" s="1"/>
+      <c r="G465" s="1"/>
+    </row>
+    <row r="466" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A466" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B466" s="1"/>
+      <c r="C466" s="1"/>
+      <c r="D466" s="1"/>
+      <c r="E466" s="1"/>
+      <c r="F466" s="1"/>
+      <c r="G466" s="1"/>
+    </row>
+    <row r="467" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A467" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B467" s="1"/>
+      <c r="C467" s="1"/>
+      <c r="D467" s="1"/>
+      <c r="E467" s="1"/>
+      <c r="F467" s="1"/>
+      <c r="G467" s="1"/>
+    </row>
+    <row r="468" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A468" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B468" s="1"/>
+      <c r="C468" s="1"/>
+      <c r="D468" s="1"/>
+      <c r="E468" s="1"/>
+      <c r="F468" s="1"/>
+      <c r="G468" s="1"/>
+    </row>
+    <row r="469" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A469" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B469" s="1"/>
+      <c r="C469" s="1"/>
+      <c r="D469" s="1"/>
+      <c r="E469" s="1"/>
+      <c r="F469" s="1"/>
+      <c r="G469" s="1"/>
+    </row>
+    <row r="470" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A470" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B470" s="1"/>
+      <c r="C470" s="1"/>
+      <c r="D470" s="1"/>
+      <c r="E470" s="1"/>
+      <c r="F470" s="1"/>
+      <c r="G470" s="1"/>
+    </row>
+    <row r="471" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A471" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B471" s="1"/>
+      <c r="C471" s="1"/>
+      <c r="D471" s="1"/>
+      <c r="E471" s="1"/>
+      <c r="F471" s="1"/>
+      <c r="G471" s="1"/>
+    </row>
+    <row r="472" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A472" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B472" s="1"/>
+      <c r="C472" s="1"/>
+      <c r="D472" s="1"/>
+      <c r="E472" s="1"/>
+      <c r="F472" s="1"/>
+      <c r="G472" s="1"/>
+    </row>
+    <row r="473" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A473" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B473" s="1"/>
+      <c r="C473" s="1"/>
+      <c r="D473" s="1"/>
+      <c r="E473" s="1"/>
+      <c r="F473" s="1"/>
+      <c r="G473" s="1"/>
+    </row>
+    <row r="474" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A474" s="1"/>
+      <c r="B474" s="1"/>
+      <c r="C474" s="1"/>
+      <c r="D474" s="1"/>
+      <c r="E474" s="1"/>
+      <c r="F474" s="1"/>
+      <c r="G474" s="1"/>
+    </row>
+    <row r="475" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A475" s="1"/>
+      <c r="B475" s="1"/>
+      <c r="C475" s="1"/>
+      <c r="D475" s="1"/>
+      <c r="E475" s="1"/>
+      <c r="F475" s="1"/>
+      <c r="G475" s="1"/>
+    </row>
+    <row r="476" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A476" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B476" s="1"/>
+      <c r="C476" s="1"/>
+      <c r="D476" s="1"/>
+      <c r="E476" s="1"/>
+      <c r="F476" s="1"/>
+      <c r="G476" s="1"/>
+    </row>
+    <row r="477" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A477" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B477" s="1"/>
+      <c r="C477" s="1"/>
+      <c r="D477" s="1"/>
+      <c r="E477" s="1"/>
+      <c r="F477" s="1"/>
+      <c r="G477" s="1"/>
+    </row>
+    <row r="478" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A478" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B478" s="1"/>
+      <c r="C478" s="1"/>
+      <c r="D478" s="1"/>
+      <c r="E478" s="1"/>
+      <c r="F478" s="1"/>
+      <c r="G478" s="1"/>
+    </row>
+    <row r="479" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A479" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B479" s="1"/>
+      <c r="C479" s="1"/>
+      <c r="D479" s="1"/>
+      <c r="E479" s="1"/>
+      <c r="F479" s="1"/>
+      <c r="G479" s="1"/>
+    </row>
+    <row r="480" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A480" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B480" s="1"/>
+      <c r="C480" s="1"/>
+      <c r="D480" s="1"/>
+      <c r="E480" s="1"/>
+      <c r="F480" s="1"/>
+      <c r="G480" s="1"/>
+    </row>
+    <row r="481" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A481" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B481" s="1"/>
+      <c r="C481" s="1"/>
+      <c r="D481" s="1"/>
+      <c r="E481" s="1"/>
+      <c r="F481" s="1"/>
+      <c r="G481" s="1"/>
+    </row>
+    <row r="482" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A482" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B482" s="1"/>
+      <c r="C482" s="1"/>
+      <c r="D482" s="1"/>
+      <c r="E482" s="1"/>
+      <c r="F482" s="1"/>
+      <c r="G482" s="1"/>
+    </row>
+    <row r="483" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A483" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B483" s="1"/>
+      <c r="C483" s="1"/>
+      <c r="D483" s="1"/>
+      <c r="E483" s="1"/>
+      <c r="F483" s="1"/>
+      <c r="G483" s="1"/>
+    </row>
+    <row r="484" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A484" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B484" s="1"/>
+      <c r="C484" s="1"/>
+      <c r="D484" s="1"/>
+      <c r="E484" s="1"/>
+      <c r="F484" s="1"/>
+      <c r="G484" s="1"/>
+    </row>
+    <row r="485" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A485" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B485" s="1"/>
+      <c r="C485" s="1"/>
+      <c r="D485" s="1"/>
+      <c r="E485" s="1"/>
+      <c r="F485" s="1"/>
+      <c r="G485" s="1"/>
+    </row>
+    <row r="486" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A486" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B486" s="1"/>
+      <c r="C486" s="1"/>
+      <c r="D486" s="1"/>
+      <c r="E486" s="1"/>
+      <c r="F486" s="1"/>
+      <c r="G486" s="1"/>
+    </row>
+    <row r="487" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A487" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B487" s="1"/>
+      <c r="C487" s="1"/>
+      <c r="D487" s="1"/>
+      <c r="E487" s="1"/>
+      <c r="F487" s="1"/>
+      <c r="G487" s="1"/>
+    </row>
+    <row r="488" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A488" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B488" s="1"/>
+      <c r="C488" s="1"/>
+      <c r="D488" s="1"/>
+      <c r="E488" s="1"/>
+      <c r="F488" s="1"/>
+      <c r="G488" s="1"/>
+    </row>
+    <row r="489" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A489" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B489" s="1"/>
+      <c r="C489" s="1"/>
+      <c r="D489" s="1"/>
+      <c r="E489" s="1"/>
+      <c r="F489" s="1"/>
+      <c r="G489" s="1"/>
+    </row>
+    <row r="490" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A490" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B490" s="1"/>
+      <c r="C490" s="1"/>
+      <c r="D490" s="1"/>
+      <c r="E490" s="1"/>
+      <c r="F490" s="1"/>
+      <c r="G490" s="1"/>
+    </row>
+    <row r="491" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A491" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B491" s="1"/>
+      <c r="C491" s="1"/>
+      <c r="D491" s="1"/>
+      <c r="E491" s="1"/>
+      <c r="F491" s="1"/>
+      <c r="G491" s="1"/>
+    </row>
+    <row r="492" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A492" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B492" s="1"/>
+      <c r="C492" s="1"/>
+      <c r="D492" s="1"/>
+      <c r="E492" s="1"/>
+      <c r="F492" s="1"/>
+      <c r="G492" s="1"/>
+    </row>
+    <row r="493" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A493" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B493" s="1"/>
+      <c r="C493" s="1"/>
+      <c r="D493" s="1"/>
+      <c r="E493" s="1"/>
+      <c r="F493" s="1"/>
+      <c r="G493" s="1"/>
+    </row>
+    <row r="494" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A494" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B494" s="1"/>
+      <c r="C494" s="1"/>
+      <c r="D494" s="1"/>
+      <c r="E494" s="1"/>
+      <c r="F494" s="1"/>
+      <c r="G494" s="1"/>
+    </row>
+    <row r="495" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A495" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B495" s="1"/>
+      <c r="C495" s="1"/>
+      <c r="D495" s="1"/>
+      <c r="E495" s="1"/>
+      <c r="F495" s="1"/>
+      <c r="G495" s="1"/>
+    </row>
+    <row r="496" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A496" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B496" s="1"/>
+      <c r="C496" s="1"/>
+      <c r="D496" s="1"/>
+      <c r="E496" s="1"/>
+      <c r="F496" s="1"/>
+      <c r="G496" s="1"/>
+    </row>
+    <row r="497" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A497" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B497" s="1"/>
+      <c r="C497" s="1"/>
+      <c r="D497" s="1"/>
+      <c r="E497" s="1"/>
+      <c r="F497" s="1"/>
+      <c r="G497" s="1"/>
+    </row>
+    <row r="498" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A498" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B498" s="1"/>
+      <c r="C498" s="1"/>
+      <c r="D498" s="1"/>
+      <c r="E498" s="1"/>
+      <c r="F498" s="1"/>
+      <c r="G498" s="1"/>
+    </row>
+    <row r="499" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A499" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B499" s="1"/>
+      <c r="C499" s="1"/>
+      <c r="D499" s="1"/>
+      <c r="E499" s="1"/>
+      <c r="F499" s="1"/>
+      <c r="G499" s="1"/>
+    </row>
+    <row r="500" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A500" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B500" s="1"/>
+      <c r="C500" s="1"/>
+      <c r="D500" s="1"/>
+      <c r="E500" s="1"/>
+      <c r="F500" s="1"/>
+      <c r="G500" s="1"/>
+    </row>
+    <row r="501" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A501" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B501" s="1"/>
+      <c r="C501" s="1"/>
+      <c r="D501" s="1"/>
+      <c r="E501" s="1"/>
+      <c r="F501" s="1"/>
+      <c r="G501" s="1"/>
+    </row>
+    <row r="502" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A502" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B502" s="1"/>
+      <c r="C502" s="1"/>
+      <c r="D502" s="1"/>
+      <c r="E502" s="1"/>
+      <c r="F502" s="1"/>
+      <c r="G502" s="1"/>
+    </row>
+    <row r="503" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A503" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B503" s="1"/>
+      <c r="C503" s="1"/>
+      <c r="D503" s="1"/>
+      <c r="E503" s="1"/>
+      <c r="F503" s="1"/>
+      <c r="G503" s="1"/>
+    </row>
+    <row r="504" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B504" s="1"/>
+      <c r="C504" s="1"/>
+      <c r="D504" s="1"/>
+      <c r="E504" s="1"/>
+      <c r="F504" s="1"/>
+      <c r="G504" s="1"/>
+    </row>
+    <row r="505" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A505" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B505" s="1"/>
+      <c r="C505" s="1"/>
+      <c r="D505" s="1"/>
+      <c r="E505" s="1"/>
+      <c r="F505" s="1"/>
+      <c r="G505" s="1"/>
+    </row>
+    <row r="506" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B506" s="1"/>
+      <c r="C506" s="1"/>
+      <c r="D506" s="1"/>
+      <c r="E506" s="1"/>
+      <c r="F506" s="1"/>
+      <c r="G506" s="1"/>
+    </row>
+    <row r="507" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A507" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B507" s="1"/>
+      <c r="C507" s="1"/>
+      <c r="D507" s="1"/>
+      <c r="E507" s="1"/>
+      <c r="F507" s="1"/>
+      <c r="G507" s="1"/>
+    </row>
+    <row r="508" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A508" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B508" s="1"/>
+      <c r="C508" s="1"/>
+      <c r="D508" s="1"/>
+      <c r="E508" s="1"/>
+      <c r="F508" s="1"/>
+      <c r="G508" s="1"/>
+    </row>
+    <row r="509" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B509" s="1"/>
+      <c r="C509" s="1"/>
+      <c r="D509" s="1"/>
+      <c r="E509" s="1"/>
+      <c r="F509" s="1"/>
+      <c r="G509" s="1"/>
+    </row>
+    <row r="510" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B510" s="1"/>
+      <c r="C510" s="1"/>
+      <c r="D510" s="1"/>
+      <c r="E510" s="1"/>
+      <c r="F510" s="1"/>
+      <c r="G510" s="1"/>
+    </row>
+    <row r="511" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B511" s="1"/>
+      <c r="C511" s="1"/>
+      <c r="D511" s="1"/>
+      <c r="E511" s="1"/>
+      <c r="F511" s="1"/>
+      <c r="G511" s="1"/>
+    </row>
+    <row r="512" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A512" s="1"/>
+      <c r="B512" s="1"/>
+      <c r="C512" s="1"/>
+      <c r="D512" s="1"/>
+      <c r="E512" s="1"/>
+      <c r="F512" s="1"/>
+      <c r="G512" s="1"/>
+    </row>
+    <row r="513" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A513" s="1"/>
+      <c r="B513" s="1"/>
+      <c r="C513" s="1"/>
+      <c r="D513" s="1"/>
+      <c r="E513" s="1"/>
+      <c r="F513" s="1"/>
+      <c r="G513" s="1"/>
+    </row>
+    <row r="514" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A514" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B514" s="1"/>
+      <c r="C514" s="1"/>
+      <c r="D514" s="1"/>
+      <c r="E514" s="1"/>
+      <c r="F514" s="1"/>
+      <c r="G514" s="1"/>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A515" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B515" s="1"/>
+      <c r="C515" s="1"/>
+      <c r="D515" s="1"/>
+      <c r="E515" s="1"/>
+      <c r="F515" s="1"/>
+      <c r="G515" s="1"/>
+    </row>
+    <row r="516" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A516" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B516" s="1"/>
+      <c r="C516" s="1"/>
+      <c r="D516" s="1"/>
+      <c r="E516" s="1"/>
+      <c r="F516" s="1"/>
+      <c r="G516" s="1"/>
+    </row>
+    <row r="517" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A517" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B517" s="1"/>
+      <c r="C517" s="1"/>
+      <c r="D517" s="1"/>
+      <c r="E517" s="1"/>
+      <c r="F517" s="1"/>
+      <c r="G517" s="1"/>
+    </row>
+    <row r="518" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A518" s="1"/>
+      <c r="B518" s="1"/>
+      <c r="C518" s="1"/>
+      <c r="D518" s="1"/>
+      <c r="E518" s="1"/>
+      <c r="F518" s="1"/>
+      <c r="G518" s="1"/>
+    </row>
+    <row r="519" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A519" s="1"/>
+      <c r="B519" s="1"/>
+      <c r="C519" s="1"/>
+      <c r="D519" s="1"/>
+      <c r="E519" s="1"/>
+      <c r="F519" s="1"/>
+      <c r="G519" s="1"/>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A520" s="1"/>
+      <c r="B520" s="1"/>
+      <c r="C520" s="1"/>
+      <c r="D520" s="1"/>
+      <c r="E520" s="1"/>
+      <c r="F520" s="1"/>
+      <c r="G520" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A440:G440"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A105:G105"/>
+    <mergeCell ref="A140:G140"/>
     <mergeCell ref="A258:G258"/>
     <mergeCell ref="A259:C259"/>
     <mergeCell ref="A284:C284"/>
     <mergeCell ref="A383:G383"/>
     <mergeCell ref="A172:G172"/>
     <mergeCell ref="A218:G218"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A105:G105"/>
-    <mergeCell ref="A140:G140"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>